<commit_message>
Hodoscope triggering and global event watch functionality, first attempt.
</commit_message>
<xml_diff>
--- a/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
+++ b/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Interfaces " sheetId="1" r:id="rId1"/>
     <sheet name="PC Command Packets" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Functionality Checklist" sheetId="4" r:id="rId3"/>
+    <sheet name="Register" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="172">
   <si>
     <t>Ethernet Module: Gigabit Transciever Interface</t>
   </si>
@@ -198,9 +200,6 @@
     <t>0x00BE11E2</t>
   </si>
   <si>
-    <t>SCROD Register Command (single command)</t>
-  </si>
-  <si>
     <t>packet size</t>
   </si>
   <si>
@@ -210,15 +209,6 @@
     <t>0x00</t>
   </si>
   <si>
-    <t>0x00A5</t>
-  </si>
-  <si>
-    <t>0x0000</t>
-  </si>
-  <si>
-    <t>Device num: SCROD RevA5 has ID "0"</t>
-  </si>
-  <si>
     <t>verbosity (31:24)</t>
   </si>
   <si>
@@ -231,15 +221,9 @@
     <t xml:space="preserve">command type </t>
   </si>
   <si>
-    <t xml:space="preserve">Ping: 0x70696e67, read: 0x72656164, write: 0x72697465 </t>
-  </si>
-  <si>
     <t>register address</t>
   </si>
   <si>
-    <t>Command data (skip for ping command)</t>
-  </si>
-  <si>
     <t>command checksum</t>
   </si>
   <si>
@@ -258,12 +242,6 @@
     <t>sum of entire words 0 to 7</t>
   </si>
   <si>
-    <t>(Read) 0x0000 or                            (Write) register value</t>
-  </si>
-  <si>
-    <t>Daughtercard Register Command</t>
-  </si>
-  <si>
     <t>Labels packet as a Register Command</t>
   </si>
   <si>
@@ -357,10 +335,233 @@
     <t>dc_RespValid</t>
   </si>
   <si>
-    <t>DC#</t>
-  </si>
-  <si>
-    <t>0x00DC</t>
+    <t>Test date</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>SCROD- HMB Register test: Trial 1</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>working?</t>
+  </si>
+  <si>
+    <t>Ping QBLink</t>
+  </si>
+  <si>
+    <t>QBLink synced</t>
+  </si>
+  <si>
+    <t>Write to SCROD Reg</t>
+  </si>
+  <si>
+    <t>Read Scrod Reg</t>
+  </si>
+  <si>
+    <t>Write to DC Reg</t>
+  </si>
+  <si>
+    <t>Read DC Reg</t>
+  </si>
+  <si>
+    <t>Register Value                                     (0x0000 for read operations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command data </t>
+  </si>
+  <si>
+    <t>packet type: device configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x70696e67</t>
+  </si>
+  <si>
+    <t>Command Type: Ping</t>
+  </si>
+  <si>
+    <t>Device label</t>
+  </si>
+  <si>
+    <t>Device #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device labels: (SCROD) 0x00A5,            (DC) 0x00DC | Device  #: 0x00 (SCROD), 0x01 through 0x08 (DC #) </t>
+  </si>
+  <si>
+    <t>Table 1. Register Command Packets</t>
+  </si>
+  <si>
+    <t>Table 2. Ping Command packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read: 0x72656164, Write: 0x72697465 </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Reg #</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>bits</t>
+  </si>
+  <si>
+    <t>11 downto 0</t>
+  </si>
+  <si>
+    <t>4 downto 0</t>
+  </si>
+  <si>
+    <t>15 downto 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 downto 0 </t>
+  </si>
+  <si>
+    <t>tx_dac_reg_data</t>
+  </si>
+  <si>
+    <t>tx_dac_load_period</t>
+  </si>
+  <si>
+    <t>tx_dac_latch_period</t>
+  </si>
+  <si>
+    <t>3 downto 0</t>
+  </si>
+  <si>
+    <t>8 downto 0</t>
+  </si>
+  <si>
+    <t>number of windows to readout</t>
+  </si>
+  <si>
+    <t>mppc dac voltage</t>
+  </si>
+  <si>
+    <t>mppc dac address on TargetX</t>
+  </si>
+  <si>
+    <t>0, 4</t>
+  </si>
+  <si>
+    <t>TargetX control reset, enables calibration</t>
+  </si>
+  <si>
+    <t>software Trigger (not implemented)</t>
+  </si>
+  <si>
+    <t>Trigger Mode (not implemented)</t>
+  </si>
+  <si>
+    <t>not used</t>
+  </si>
+  <si>
+    <t>Daughtercard FPGA Control Registers</t>
+  </si>
+  <si>
+    <t>1/2 trigger scalar count (not implemented)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2/2 trigger scalar count</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(not implemented)</t>
+    </r>
+  </si>
+  <si>
+    <t>trigger count enable(not implemented)</t>
+  </si>
+  <si>
+    <t>maximum trigger count (not implemented)</t>
+  </si>
+  <si>
+    <t>Resets stamachines</t>
+  </si>
+  <si>
+    <t>SCROD ID</t>
+  </si>
+  <si>
+    <t>dc_mask (not implemented)</t>
+  </si>
+  <si>
+    <t>output mode (not implemented)</t>
+  </si>
+  <si>
+    <t>15, 3 downto 0</t>
+  </si>
+  <si>
+    <t>enable pedestal subtraction, number of averages for calculating peds (1-7)</t>
+  </si>
+  <si>
+    <t>resets  window number during sampling, sets timing for sstin and current window count in targetX</t>
+  </si>
+  <si>
+    <t>15, 1 downto 0</t>
+  </si>
+  <si>
+    <t>sets wait period for digitizing ramp</t>
+  </si>
+  <si>
+    <t>15, 8 downto 0</t>
+  </si>
+  <si>
+    <t>enable use of fixed window, fixed start window</t>
+  </si>
+  <si>
+    <t>15, 8 downt 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SCROD acknowledgement wait</t>
+  </si>
+  <si>
+    <t>offset window direcion, number of windows to offset</t>
+  </si>
+  <si>
+    <t>SCROD FPGA Control Registers</t>
+  </si>
+  <si>
+    <t>broad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device labels: (SCROD) 0x00A5,            (DC) 0x00DC | Device  #: 0x00 (SCROD), 0x01 through 0x08 (DC #) or 0x0A for broadcasting to all DCs. </t>
+  </si>
+  <si>
+    <t>0, 8* downto 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync Daughtercards, reset QBLink (*msb depends on how many DC you have) </t>
   </si>
 </sst>
 </file>
@@ -532,7 +733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1086,11 +1287,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1230,8 +1526,141 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1258,6 +1687,56 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1267,9 +1746,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1279,138 +1768,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1730,19 +2098,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57"/>
+      <c r="C2" s="112"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="53"/>
+      <c r="C3" s="108"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="2:6">
@@ -1782,10 +2150,10 @@
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="53"/>
+      <c r="C8" s="108"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="2:6">
@@ -1813,16 +2181,16 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="112"/>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="108"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="2" t="s">
@@ -1865,10 +2233,10 @@
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="55"/>
+      <c r="C21" s="110"/>
     </row>
     <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="17" t="s">
@@ -1913,16 +2281,16 @@
     <row r="27" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="28" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="29" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B29" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="57"/>
+      <c r="B29" s="114" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="112"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="55"/>
+      <c r="C30" s="110"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" customHeight="1">
       <c r="B31" s="2" t="s">
@@ -1949,10 +2317,10 @@
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="55"/>
+      <c r="C34" s="110"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="15" t="s">
@@ -1971,10 +2339,10 @@
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="55"/>
+      <c r="C37" s="110"/>
     </row>
     <row r="38" spans="2:3" ht="15.75" customHeight="1">
       <c r="B38" s="24" t="s">
@@ -2011,167 +2379,167 @@
     <row r="42" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="43" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B44" s="101" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="57"/>
+      <c r="B44" s="118" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="112"/>
     </row>
     <row r="45" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="121" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="122"/>
+    </row>
+    <row r="46" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B46" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B47" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B48" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" s="40" customFormat="1" ht="30" customHeight="1">
+      <c r="B49" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B50" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B51" s="123" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="124"/>
+    </row>
+    <row r="52" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B52" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B53" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B54" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="81"/>
-    </row>
-    <row r="46" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B46" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="83" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B47" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="85" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B48" s="86" t="s">
+    </row>
+    <row r="55" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B55" s="125" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="126"/>
+    </row>
+    <row r="56" spans="2:3" ht="30" customHeight="1">
+      <c r="B56" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="87" t="s">
+    </row>
+    <row r="57" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B57" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="64" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" s="40" customFormat="1" ht="30" customHeight="1">
-      <c r="B49" s="86" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" s="87" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B50" s="116" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" s="88" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B51" s="89" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="90"/>
-    </row>
-    <row r="52" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B52" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="92" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B53" s="93" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="94" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B54" s="93" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="94" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B55" s="95" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="99"/>
-    </row>
-    <row r="56" spans="2:3" ht="30" customHeight="1">
-      <c r="B56" s="96" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="97" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B57" s="100" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="98" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="59" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="60" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B60" s="114" t="s">
+      <c r="B60" s="127" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="128"/>
+    </row>
+    <row r="61" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B61" s="129" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="130"/>
+    </row>
+    <row r="62" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B62" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B63" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="69" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B64" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B65" s="119" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="120"/>
+    </row>
+    <row r="66" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B66" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B67" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" s="73" t="s">
         <v>100</v>
-      </c>
-      <c r="C60" s="115"/>
-    </row>
-    <row r="61" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B61" s="102" t="s">
-        <v>101</v>
-      </c>
-      <c r="C61" s="103"/>
-    </row>
-    <row r="62" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B62" s="104" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="105" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B63" s="106" t="s">
-        <v>104</v>
-      </c>
-      <c r="C63" s="107" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B64" s="106" t="s">
-        <v>103</v>
-      </c>
-      <c r="C64" s="107" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B65" s="108" t="s">
-        <v>106</v>
-      </c>
-      <c r="C65" s="109"/>
-    </row>
-    <row r="66" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B66" s="110" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="111" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B67" s="112" t="s">
-        <v>107</v>
-      </c>
-      <c r="C67" s="113" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="15.75" customHeight="1"/>
@@ -3136,10 +3504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F1000"/>
+  <dimension ref="A2:M999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3154,31 +3522,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
+      <c r="B2" s="141" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="143"/>
+      <c r="D3" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="70" t="s">
+      <c r="E3" s="143"/>
+      <c r="F3" s="139" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="77"/>
+      <c r="A4" s="132"/>
       <c r="B4" s="41" t="s">
         <v>55</v>
       </c>
@@ -3191,66 +3559,66 @@
       <c r="E4" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="71"/>
+      <c r="F4" s="140"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="45">
         <v>0</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="135"/>
       <c r="F5" s="46" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1">
       <c r="A6" s="45">
         <v>1</v>
       </c>
-      <c r="B6" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="74"/>
+      <c r="B6" s="133" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="135"/>
       <c r="F6" s="47" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="45">
         <v>2</v>
       </c>
-      <c r="B7" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="74"/>
+      <c r="B7" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="135"/>
       <c r="F7" s="47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="75" customFormat="1" ht="84.75" customHeight="1">
       <c r="A8" s="45">
         <v>3</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="74"/>
+        <v>62</v>
+      </c>
+      <c r="C8" s="133" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="135"/>
       <c r="E8" s="42" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" customHeight="1">
@@ -3258,259 +3626,248 @@
         <v>4</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
+        <v>63</v>
+      </c>
+      <c r="C9" s="136" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="137"/>
+      <c r="E9" s="138"/>
       <c r="F9" s="47" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1">
       <c r="A10" s="45">
         <v>5</v>
       </c>
-      <c r="B10" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
+      <c r="B10" s="136" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="137"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="138"/>
       <c r="F10" s="48" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1">
       <c r="A11" s="45">
         <v>6</v>
       </c>
-      <c r="B11" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="65"/>
+      <c r="B11" s="136" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="138"/>
+      <c r="D11" s="142" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="138"/>
       <c r="F11" s="48" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="45">
         <v>7</v>
       </c>
-      <c r="B12" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
+      <c r="B12" s="136" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="137"/>
+      <c r="D12" s="137"/>
+      <c r="E12" s="138"/>
       <c r="F12" s="48" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1">
       <c r="A13" s="49">
         <v>8</v>
       </c>
-      <c r="B13" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="69"/>
+      <c r="B13" s="144" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="145"/>
+      <c r="D13" s="145"/>
+      <c r="E13" s="146"/>
       <c r="F13" s="50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B15" s="75" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
-      <c r="A16" s="76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A16" s="75"/>
+      <c r="B16" s="141" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="141"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="75"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1">
+      <c r="A17" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B17" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78" t="s">
+      <c r="C17" s="143"/>
+      <c r="D17" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="78"/>
-      <c r="F16" s="70" t="s">
+      <c r="E17" s="143"/>
+      <c r="F17" s="139" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
-      <c r="A17" s="77"/>
-      <c r="B17" s="41" t="s">
+    <row r="18" spans="1:13" ht="15" customHeight="1">
+      <c r="A18" s="132"/>
+      <c r="B18" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C18" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D18" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E18" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="71"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="45">
+      <c r="F18" s="140"/>
+    </row>
+    <row r="19" spans="1:13" s="44" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="45">
         <v>0</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B19" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="46" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="44" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="51">
+      <c r="C19" s="134"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="44" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="45">
         <v>1</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B20" s="133" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A21" s="45">
+        <v>2</v>
+      </c>
+      <c r="B21" s="133" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="51">
-        <v>2</v>
-      </c>
-      <c r="B20" s="63" t="s">
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="135"/>
+      <c r="F21" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="45" customHeight="1">
+      <c r="A22" s="45">
+        <v>3</v>
+      </c>
+      <c r="B22" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="45">
-        <v>3</v>
-      </c>
-      <c r="B21" s="42" t="s">
+      <c r="C22" s="133" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="135"/>
+      <c r="E22" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" customHeight="1">
+      <c r="A23" s="45">
+        <v>4</v>
+      </c>
+      <c r="B23" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1">
-      <c r="A22" s="45">
-        <v>4</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="63" t="s">
+      <c r="C23" s="136" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="137"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="90" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" customHeight="1">
+      <c r="A24" s="45">
+        <v>5</v>
+      </c>
+      <c r="B24" s="136" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="M24" s="91" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A25" s="45">
+        <v>6</v>
+      </c>
+      <c r="B25" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="47" t="s">
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A26" s="49">
+        <v>7</v>
+      </c>
+      <c r="B26" s="144" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1">
-      <c r="A23" s="45">
-        <v>5</v>
-      </c>
-      <c r="B23" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="45">
-        <v>6</v>
-      </c>
-      <c r="B24" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="66" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="65"/>
-      <c r="F24" s="48" t="s">
+      <c r="C26" s="145"/>
+      <c r="D26" s="145"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="50" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A25" s="45">
-        <v>7</v>
-      </c>
-      <c r="B25" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="49">
-        <v>8</v>
-      </c>
-      <c r="B26" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="33" ht="30" customHeight="1"/>
+    <row r="34" ht="30" customHeight="1"/>
+    <row r="35" ht="47.25" customHeight="1"/>
+    <row r="36" ht="30.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -4474,9 +4831,20 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="28">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B19:E19"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B2:E2"/>
@@ -4484,29 +4852,15 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4515,12 +4869,723 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:3">
+      <c r="B3" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="30.75" thickBot="1">
+      <c r="B4" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="88">
+        <v>43579</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B5" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="86" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="83" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="84" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="79"/>
+      <c r="C12" s="80"/>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="79"/>
+      <c r="C14" s="80"/>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="79"/>
+      <c r="C18" s="80"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="79"/>
+      <c r="C21" s="80"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="79"/>
+      <c r="C23" s="80"/>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="79"/>
+      <c r="C24" s="80"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="79"/>
+      <c r="C25" s="80"/>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="79"/>
+      <c r="C26" s="80"/>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="79"/>
+      <c r="C27" s="80"/>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="79"/>
+      <c r="C28" s="80"/>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="79"/>
+      <c r="C29" s="80"/>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="79"/>
+      <c r="C30" s="80"/>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="79"/>
+      <c r="C31" s="80"/>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B32" s="81"/>
+      <c r="C32" s="82"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P17" sqref="P16:P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="55" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="51.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="19.5" thickBot="1">
+      <c r="B2" s="147" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="G2" s="149" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="98" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="99" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="100" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="98" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="99" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="100" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="45">
+        <v>0</v>
+      </c>
+      <c r="C4" s="92" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="93" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="104">
+        <v>0</v>
+      </c>
+      <c r="H4" s="105">
+        <v>0</v>
+      </c>
+      <c r="I4" s="106" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="45">
+        <v>1</v>
+      </c>
+      <c r="C5" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="45">
+        <v>1</v>
+      </c>
+      <c r="H5" s="94">
+        <v>0</v>
+      </c>
+      <c r="I5" s="93" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="30">
+      <c r="B6" s="45">
+        <v>2</v>
+      </c>
+      <c r="C6" s="92" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="45">
+        <v>2</v>
+      </c>
+      <c r="H6" s="92" t="s">
+        <v>170</v>
+      </c>
+      <c r="I6" s="47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="45">
+        <v>3</v>
+      </c>
+      <c r="C7" s="92" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="93" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="45">
+        <v>3</v>
+      </c>
+      <c r="H7" s="94"/>
+      <c r="I7" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="45">
+        <v>4</v>
+      </c>
+      <c r="C8" s="92" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="93" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="45">
+        <v>4</v>
+      </c>
+      <c r="H8" s="94"/>
+      <c r="I8" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="45">
+        <v>5</v>
+      </c>
+      <c r="C9" s="94">
+        <v>0</v>
+      </c>
+      <c r="D9" s="95" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="45">
+        <v>5</v>
+      </c>
+      <c r="H9" s="94">
+        <v>0</v>
+      </c>
+      <c r="I9" s="95" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="45">
+        <v>6</v>
+      </c>
+      <c r="C10" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="95" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="45">
+        <v>6</v>
+      </c>
+      <c r="H10" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="I10" s="95" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="45">
+        <v>7</v>
+      </c>
+      <c r="C11" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="45">
+        <v>7</v>
+      </c>
+      <c r="H11" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" s="95" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="45">
+        <v>8</v>
+      </c>
+      <c r="C12" s="92" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="93" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="45">
+        <v>8</v>
+      </c>
+      <c r="H12" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="I12" s="95" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="45">
+        <v>9</v>
+      </c>
+      <c r="C13" s="92" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="93" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="45">
+        <v>9</v>
+      </c>
+      <c r="H13" s="94"/>
+      <c r="I13" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="45">
+        <v>10</v>
+      </c>
+      <c r="C14" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="93" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="45">
+        <v>10</v>
+      </c>
+      <c r="H14" s="94"/>
+      <c r="I14" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="45">
+        <v>11</v>
+      </c>
+      <c r="C15" s="92" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="95" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="45">
+        <v>11</v>
+      </c>
+      <c r="H15" s="94"/>
+      <c r="I15" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="45">
+        <v>12</v>
+      </c>
+      <c r="C16" s="92" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="93" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="45">
+        <v>12</v>
+      </c>
+      <c r="H16" s="92" t="s">
+        <v>162</v>
+      </c>
+      <c r="I16" s="93" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="30">
+      <c r="B17" s="45">
+        <v>13</v>
+      </c>
+      <c r="C17" s="92" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="45">
+        <v>13</v>
+      </c>
+      <c r="H17" s="94"/>
+      <c r="I17" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="30">
+      <c r="B18" s="45">
+        <v>14</v>
+      </c>
+      <c r="C18" s="92" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="45">
+        <v>14</v>
+      </c>
+      <c r="H18" s="94"/>
+      <c r="I18" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="45">
+        <v>15</v>
+      </c>
+      <c r="C19" s="103"/>
+      <c r="D19" s="93" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="45">
+        <v>15</v>
+      </c>
+      <c r="H19" s="94"/>
+      <c r="I19" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="45">
+        <v>16</v>
+      </c>
+      <c r="C20" s="94"/>
+      <c r="D20" s="93" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="45">
+        <v>16</v>
+      </c>
+      <c r="H20" s="94"/>
+      <c r="I20" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="45">
+        <v>17</v>
+      </c>
+      <c r="C21" s="92"/>
+      <c r="D21" s="93" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="45">
+        <v>17</v>
+      </c>
+      <c r="H21" s="94"/>
+      <c r="I21" s="95" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="45">
+        <v>18</v>
+      </c>
+      <c r="C22" s="94" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="45">
+        <v>18</v>
+      </c>
+      <c r="H22" s="94" t="s">
+        <v>132</v>
+      </c>
+      <c r="I22" s="95" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="45">
+        <v>19</v>
+      </c>
+      <c r="C23" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="45">
+        <v>19</v>
+      </c>
+      <c r="H23" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" s="95" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="45">
+        <v>20</v>
+      </c>
+      <c r="C24" s="94" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="45">
+        <v>20</v>
+      </c>
+      <c r="H24" s="94" t="s">
+        <v>133</v>
+      </c>
+      <c r="I24" s="93" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B25" s="49">
+        <v>21</v>
+      </c>
+      <c r="C25" s="96">
+        <v>0</v>
+      </c>
+      <c r="D25" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="49">
+        <v>21</v>
+      </c>
+      <c r="H25" s="96">
+        <v>0</v>
+      </c>
+      <c r="I25" s="97" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="102"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="101"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="102"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="101"/>
+      <c r="H27" s="101"/>
+      <c r="I27" s="101"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="102"/>
+      <c r="C28" s="102"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="101"/>
+    </row>
+  </sheetData>
+  <sortState ref="B4:G27">
+    <sortCondition ref="B4:B27"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expand SCROD register process sensitity list to includ all flags.
</commit_message>
<xml_diff>
--- a/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
+++ b/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interfaces " sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="171">
   <si>
     <t>Ethernet Module: Gigabit Transciever Interface</t>
   </si>
@@ -552,16 +552,13 @@
     <t>SCROD FPGA Control Registers</t>
   </si>
   <si>
-    <t>broad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Device labels: (SCROD) 0x00A5,            (DC) 0x00DC | Device  #: 0x00 (SCROD), 0x01 through 0x08 (DC #) or 0x0A for broadcasting to all DCs. </t>
   </si>
   <si>
-    <t>0, 8* downto 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sync Daughtercards, reset QBLink (*msb depends on how many DC you have) </t>
+  </si>
+  <si>
+    <t>8, 7* downto 0</t>
   </si>
 </sst>
 </file>
@@ -1662,6 +1659,53 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1669,58 +1713,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1728,6 +1725,33 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1737,35 +1761,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2098,19 +2095,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="112"/>
+      <c r="C2" s="120"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="108"/>
+      <c r="C3" s="127"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="2:6">
@@ -2150,10 +2147,10 @@
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="108"/>
+      <c r="C8" s="127"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="2:6">
@@ -2181,16 +2178,16 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="112"/>
+      <c r="C14" s="120"/>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="108"/>
+      <c r="C15" s="127"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="2" t="s">
@@ -2233,10 +2230,10 @@
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="110"/>
+      <c r="C21" s="122"/>
     </row>
     <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="17" t="s">
@@ -2281,16 +2278,16 @@
     <row r="27" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="28" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="29" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B29" s="114" t="s">
+      <c r="B29" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="112"/>
+      <c r="C29" s="120"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B30" s="115" t="s">
+      <c r="B30" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="110"/>
+      <c r="C30" s="122"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" customHeight="1">
       <c r="B31" s="2" t="s">
@@ -2317,10 +2314,10 @@
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="110"/>
+      <c r="C34" s="122"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="15" t="s">
@@ -2339,10 +2336,10 @@
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B37" s="117" t="s">
+      <c r="B37" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="110"/>
+      <c r="C37" s="122"/>
     </row>
     <row r="38" spans="2:3" ht="15.75" customHeight="1">
       <c r="B38" s="24" t="s">
@@ -2379,16 +2376,16 @@
     <row r="42" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="43" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B44" s="118" t="s">
+      <c r="B44" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="112"/>
+      <c r="C44" s="120"/>
     </row>
     <row r="45" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B45" s="121" t="s">
+      <c r="B45" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="122"/>
+      <c r="C45" s="110"/>
     </row>
     <row r="46" spans="2:3" ht="15.75" customHeight="1">
       <c r="B46" s="51" t="s">
@@ -2431,10 +2428,10 @@
       </c>
     </row>
     <row r="51" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B51" s="123" t="s">
+      <c r="B51" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="124"/>
+      <c r="C51" s="112"/>
     </row>
     <row r="52" spans="2:3" ht="15.75" customHeight="1">
       <c r="B52" s="58" t="s">
@@ -2461,10 +2458,10 @@
       </c>
     </row>
     <row r="55" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B55" s="125" t="s">
+      <c r="B55" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="126"/>
+      <c r="C55" s="114"/>
     </row>
     <row r="56" spans="2:3" ht="30" customHeight="1">
       <c r="B56" s="62" t="s">
@@ -2485,16 +2482,16 @@
     <row r="58" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="59" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="60" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B60" s="127" t="s">
+      <c r="B60" s="115" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="128"/>
+      <c r="C60" s="116"/>
     </row>
     <row r="61" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B61" s="129" t="s">
+      <c r="B61" s="117" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="130"/>
+      <c r="C61" s="118"/>
     </row>
     <row r="62" spans="2:3" ht="15.75" customHeight="1">
       <c r="B62" s="66" t="s">
@@ -2521,10 +2518,10 @@
       </c>
     </row>
     <row r="65" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B65" s="119" t="s">
+      <c r="B65" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="120"/>
+      <c r="C65" s="108"/>
     </row>
     <row r="66" spans="2:3" ht="15.75" customHeight="1">
       <c r="B66" s="70" t="s">
@@ -3479,23 +3476,23 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3506,8 +3503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M999"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3522,26 +3519,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="145" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143" t="s">
+      <c r="C3" s="133"/>
+      <c r="D3" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="143"/>
-      <c r="F3" s="139" t="s">
+      <c r="E3" s="133"/>
+      <c r="F3" s="134" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3559,18 +3556,18 @@
       <c r="E4" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="140"/>
+      <c r="F4" s="135"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="45">
         <v>0</v>
       </c>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="135"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="144"/>
       <c r="F5" s="46" t="s">
         <v>71</v>
       </c>
@@ -3579,12 +3576,12 @@
       <c r="A6" s="45">
         <v>1</v>
       </c>
-      <c r="B6" s="133" t="s">
+      <c r="B6" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="135"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="144"/>
       <c r="F6" s="47" t="s">
         <v>70</v>
       </c>
@@ -3593,12 +3590,12 @@
       <c r="A7" s="45">
         <v>2</v>
       </c>
-      <c r="B7" s="133" t="s">
+      <c r="B7" s="142" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="135"/>
+      <c r="C7" s="143"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="144"/>
       <c r="F7" s="47" t="s">
         <v>74</v>
       </c>
@@ -3610,15 +3607,15 @@
       <c r="B8" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="133" t="s">
+      <c r="C8" s="142" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="135"/>
+      <c r="D8" s="144"/>
       <c r="E8" s="42" t="s">
         <v>122</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" customHeight="1">
@@ -3659,7 +3656,7 @@
         <v>116</v>
       </c>
       <c r="C11" s="138"/>
-      <c r="D11" s="142" t="s">
+      <c r="D11" s="146" t="s">
         <v>67</v>
       </c>
       <c r="E11" s="138"/>
@@ -3685,39 +3682,39 @@
       <c r="A13" s="49">
         <v>8</v>
       </c>
-      <c r="B13" s="144" t="s">
+      <c r="B13" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="145"/>
-      <c r="D13" s="145"/>
-      <c r="E13" s="146"/>
+      <c r="C13" s="140"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="141"/>
       <c r="F13" s="50" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="75"/>
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="145" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="141"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="145"/>
+      <c r="E16" s="145"/>
       <c r="F16" s="75"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1">
       <c r="A17" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="143" t="s">
+      <c r="B17" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="143"/>
-      <c r="D17" s="143" t="s">
+      <c r="C17" s="133"/>
+      <c r="D17" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="143"/>
-      <c r="F17" s="139" t="s">
+      <c r="E17" s="133"/>
+      <c r="F17" s="134" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3735,18 +3732,18 @@
       <c r="E18" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="140"/>
+      <c r="F18" s="135"/>
     </row>
     <row r="19" spans="1:13" s="44" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="45">
         <v>0</v>
       </c>
-      <c r="B19" s="133" t="s">
+      <c r="B19" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="135"/>
+      <c r="C19" s="143"/>
+      <c r="D19" s="143"/>
+      <c r="E19" s="144"/>
       <c r="F19" s="46" t="s">
         <v>71</v>
       </c>
@@ -3755,12 +3752,12 @@
       <c r="A20" s="45">
         <v>1</v>
       </c>
-      <c r="B20" s="133" t="s">
+      <c r="B20" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="135"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="143"/>
+      <c r="E20" s="144"/>
       <c r="F20" s="47" t="s">
         <v>70</v>
       </c>
@@ -3769,12 +3766,12 @@
       <c r="A21" s="45">
         <v>2</v>
       </c>
-      <c r="B21" s="133" t="s">
+      <c r="B21" s="142" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
-      <c r="E21" s="135"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="143"/>
+      <c r="E21" s="144"/>
       <c r="F21" s="48" t="s">
         <v>118</v>
       </c>
@@ -3786,10 +3783,10 @@
       <c r="B22" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="133" t="s">
+      <c r="C22" s="142" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="135"/>
+      <c r="D22" s="144"/>
       <c r="E22" s="42" t="s">
         <v>122</v>
       </c>
@@ -3826,9 +3823,7 @@
       <c r="F24" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="M24" s="91" t="s">
-        <v>168</v>
-      </c>
+      <c r="M24" s="91"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="45">
@@ -3848,12 +3843,12 @@
       <c r="A26" s="49">
         <v>7</v>
       </c>
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="145"/>
-      <c r="D26" s="145"/>
-      <c r="E26" s="146"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="141"/>
       <c r="F26" s="50" t="s">
         <v>73</v>
       </c>
@@ -4833,18 +4828,14 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B2:E2"/>
@@ -4853,14 +4844,18 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -5048,8 +5043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P17" sqref="P16:P17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5157,7 +5152,7 @@
         <v>170</v>
       </c>
       <c r="I6" s="47" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:9">

</xml_diff>

<commit_message>
Testbench of trigger data readout successful, debugging register operations.
</commit_message>
<xml_diff>
--- a/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
+++ b/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Interfaces " sheetId="1" r:id="rId1"/>
-    <sheet name="PC Command Packets" sheetId="3" r:id="rId2"/>
-    <sheet name="Functionality Checklist" sheetId="4" r:id="rId3"/>
-    <sheet name="Register" sheetId="5" r:id="rId4"/>
+    <sheet name="SCROD side Signals" sheetId="1" r:id="rId1"/>
+    <sheet name="DC side signals" sheetId="6" r:id="rId2"/>
+    <sheet name="PC Command Packets" sheetId="3" r:id="rId3"/>
+    <sheet name="Functionality Checklist" sheetId="4" r:id="rId4"/>
+    <sheet name="Register" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -18,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="171">
-  <si>
-    <t>Ethernet Module: Gigabit Transciever Interface</t>
-  </si>
-  <si>
-    <t>Register Address and Write Data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="192">
   <si>
     <t>From PC/Input Signals</t>
   </si>
@@ -35,27 +30,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>regAddr</t>
-  </si>
-  <si>
-    <t>4-bit register address</t>
-  </si>
-  <si>
-    <t>regWrData</t>
-  </si>
-  <si>
     <t xml:space="preserve">gtRx </t>
   </si>
   <si>
-    <t>16-bit register value</t>
-  </si>
-  <si>
     <t>Serial PC data in (differential)</t>
   </si>
   <si>
-    <t>Register Read Data</t>
-  </si>
-  <si>
     <t>gtClk</t>
   </si>
   <si>
@@ -71,9 +51,6 @@
     <t>To PC/Output Signals</t>
   </si>
   <si>
-    <t>regRdData</t>
-  </si>
-  <si>
     <t>current register value</t>
   </si>
   <si>
@@ -98,9 +75,6 @@
     <t>begin a register operation</t>
   </si>
   <si>
-    <t>Ethernet-Command Interpreter Interface</t>
-  </si>
-  <si>
     <t>regOp</t>
   </si>
   <si>
@@ -110,66 +84,27 @@
     <t>reset</t>
   </si>
   <si>
-    <t>Receiving Data From PC (RX)</t>
-  </si>
-  <si>
     <t>reset command from Ethernet Module</t>
   </si>
   <si>
-    <t>userRxData</t>
-  </si>
-  <si>
     <t>regAck</t>
   </si>
   <si>
     <t>Two 32-bit channels of incoming PC data</t>
   </si>
   <si>
-    <t>useRxDataValid</t>
-  </si>
-  <si>
-    <t>2-bit flag: valid incoming word</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userRxDataLast </t>
-  </si>
-  <si>
-    <t>2-bit flag: last word in incoming packet</t>
-  </si>
-  <si>
-    <t>userRxdataReady</t>
-  </si>
-  <si>
     <t>Register handshake</t>
   </si>
   <si>
-    <t>2-bit flag: Interpreter ready to receive data</t>
-  </si>
-  <si>
-    <t>Sending Data to PC (TX</t>
-  </si>
-  <si>
-    <t>userTxData</t>
-  </si>
-  <si>
     <t>Two 32-bit channels of outgoing PC Data</t>
   </si>
   <si>
-    <t>useTxDataValid</t>
-  </si>
-  <si>
     <t>2-bit flag: Valid outgoing word</t>
   </si>
   <si>
-    <t xml:space="preserve">userTxDataLast </t>
-  </si>
-  <si>
     <t xml:space="preserve">2-bit flag: last word in outgoing packet </t>
   </si>
   <si>
-    <t>userTxdataReady</t>
-  </si>
-  <si>
     <t>2-bit flag: Ethernet  ready to transmit data</t>
   </si>
   <si>
@@ -248,88 +183,16 @@
     <t>Command Interpreter-Control Register Interface</t>
   </si>
   <si>
-    <t>QB_rst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBLink reset </t>
-  </si>
-  <si>
     <t xml:space="preserve">QBLink Control Flags </t>
   </si>
   <si>
-    <t>Read output FIFO</t>
-  </si>
-  <si>
-    <t>trgLinksynced</t>
-  </si>
-  <si>
-    <t>serialClkLocked</t>
-  </si>
-  <si>
-    <t>partners clock aligned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partners synced, training state passed </t>
-  </si>
-  <si>
     <t xml:space="preserve">DC Command </t>
   </si>
   <si>
-    <t xml:space="preserve">32-bit word to be sent to DC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable write to input fifo </t>
-  </si>
-  <si>
-    <t>DC Register Data</t>
-  </si>
-  <si>
-    <t>DCResonse</t>
-  </si>
-  <si>
-    <t>32-bit response to command (non-event data)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valid Reponse </t>
-  </si>
-  <si>
-    <t>Command Interpreter-DC Communication Interface</t>
-  </si>
-  <si>
-    <t>DC Communication: QBLink Interface</t>
-  </si>
-  <si>
     <t>To DC</t>
   </si>
   <si>
-    <t>Synchronize all DC</t>
-  </si>
-  <si>
-    <t>tx_dc</t>
-  </si>
-  <si>
-    <t>sync</t>
-  </si>
-  <si>
-    <t>serial output to DC</t>
-  </si>
-  <si>
     <t>From DC</t>
-  </si>
-  <si>
-    <t>rx_dc</t>
-  </si>
-  <si>
-    <t>serial input from DC</t>
-  </si>
-  <si>
-    <t>QBstart_rd</t>
-  </si>
-  <si>
-    <t>QBstart_wr</t>
-  </si>
-  <si>
-    <t>dc_cmd</t>
   </si>
   <si>
     <t>dc_RespValid</t>
@@ -560,12 +423,213 @@
   <si>
     <t>8, 7* downto 0</t>
   </si>
+  <si>
+    <t xml:space="preserve">Synchronize all DCs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signals between Command Interpreter and DC Communication </t>
+  </si>
+  <si>
+    <t>Signals between SCROD and Daughtercards</t>
+  </si>
+  <si>
+    <t>Signals between S6 Ethernet and Command Interpreter</t>
+  </si>
+  <si>
+    <t>Signals between SCROD and Gigabit Transceiver (PC Interface)</t>
+  </si>
+  <si>
+    <t>From Ethernet (RX)</t>
+  </si>
+  <si>
+    <t>To Ethernet (TX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select target DC(s) for command </t>
+  </si>
+  <si>
+    <t>Select target DC(s) for readout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DC command Type, DC register value and address</t>
+  </si>
+  <si>
+    <t>DC Status</t>
+  </si>
+  <si>
+    <t>Valid Reponse Flag</t>
+  </si>
+  <si>
+    <t>Response to register command or trigger data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evntFlag </t>
+  </si>
+  <si>
+    <t>DCResonse(32 bits)</t>
+  </si>
+  <si>
+    <t>dc_cmd (32 bits)</t>
+  </si>
+  <si>
+    <t>Sync (8 bits)</t>
+  </si>
+  <si>
+    <t>tx_dc(8 bits)</t>
+  </si>
+  <si>
+    <t>rx_dc( 8 bits)</t>
+  </si>
+  <si>
+    <t>serial input from DCs</t>
+  </si>
+  <si>
+    <t>QBLink serial output to DCs</t>
+  </si>
+  <si>
+    <t>Qbstart_wr(8 bits)</t>
+  </si>
+  <si>
+    <t>QBstart_rd(8 bits)</t>
+  </si>
+  <si>
+    <t>trgLinksynced(8 bits)</t>
+  </si>
+  <si>
+    <t>serialClkLocked(8 bits)</t>
+  </si>
+  <si>
+    <t>QB_rst(8 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select QBLink(s) to reset </t>
+  </si>
+  <si>
+    <t>QBLink partners clock aligned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBLink partners synced, training state passed </t>
+  </si>
+  <si>
+    <t>Global Event flag</t>
+  </si>
+  <si>
+    <t>regRdData(16 bits)</t>
+  </si>
+  <si>
+    <t>regAddr (16 bits)</t>
+  </si>
+  <si>
+    <t>regWrData(16 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> register value</t>
+  </si>
+  <si>
+    <t>SCROD Register Address and Write Data</t>
+  </si>
+  <si>
+    <t>SCROD Register Read Data</t>
+  </si>
+  <si>
+    <t>register address (acceptable values: 0 to 15)</t>
+  </si>
+  <si>
+    <t>useRxDataValid(2 bits)</t>
+  </si>
+  <si>
+    <t>userRxDataLast (2 bits)</t>
+  </si>
+  <si>
+    <t>userRxdataReady (2 bits)</t>
+  </si>
+  <si>
+    <t>userTxData(2 32 bit channels)</t>
+  </si>
+  <si>
+    <t>useTxDataValid (2 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userTxDataLast (2 bits) </t>
+  </si>
+  <si>
+    <t>userTxdataReady (2 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> valid incoming word flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> last word in incoming packet flag</t>
+  </si>
+  <si>
+    <t>Interpreter ready to receive data flag</t>
+  </si>
+  <si>
+    <t>userRxData (2 32 bit channels)</t>
+  </si>
+  <si>
+    <t>Packet type error: ERR_BIT_TYPE_C = x"00000002"</t>
+  </si>
+  <si>
+    <t>Packet size error: ERR_BIT_SIZE_C = x"00000001"</t>
+  </si>
+  <si>
+    <t>Invalid command target: ERR_BIT_DEST_C = x"00000004"</t>
+  </si>
+  <si>
+    <t>Invalid command type: ERR_BIT_COMM_TY_C = x"00000008"</t>
+  </si>
+  <si>
+    <t>Command checksum error: ERR_BIT_COMM_CS_C = x"00000010"</t>
+  </si>
+  <si>
+    <t>Packet checksum error: ERR_BIT_CS_C = x"00000020"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Timeout Error: ERR_BIT_TIMEOUT_C = x"00000040"</t>
+  </si>
+  <si>
+    <t>connection to DC failed: QBLINK_FAILURE_C: x"00000500"</t>
+  </si>
+  <si>
+    <t>Error Response</t>
+  </si>
+  <si>
+    <t>word#</t>
+  </si>
+  <si>
+    <t>x"00BE11E2"</t>
+  </si>
+  <si>
+    <t>x"00000005"</t>
+  </si>
+  <si>
+    <t>word_err_c = x"7768613f"</t>
+  </si>
+  <si>
+    <t>wordScrodRevC = x"0000A500"</t>
+  </si>
+  <si>
+    <t>00 &amp; commandId</t>
+  </si>
+  <si>
+    <t>errFlags</t>
+  </si>
+  <si>
+    <t>Error constants (errflags)</t>
+  </si>
+  <si>
+    <t>checksum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -584,17 +648,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
@@ -637,8 +690,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,48 +751,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor rgb="FFC6D9F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor rgb="FFC6D9F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FFE5B8B7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor rgb="FFFBD4B4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor rgb="FFE5B8B7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -729,8 +761,56 @@
         <bgColor rgb="FFC6D9F0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE583D9"/>
+        <bgColor rgb="FFC6D9F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE583D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor rgb="FFFBD4B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor rgb="FFE5B8B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor rgb="FFE5B8B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor rgb="FFC6D9F0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="50">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1207,27 +1287,27 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1239,9 +1319,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1254,9 +1332,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1266,7 +1342,87 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1274,7 +1430,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1282,108 +1440,13 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1394,70 +1457,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1467,39 +1482,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1508,139 +1504,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1650,109 +1574,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1761,20 +1628,263 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1783,6 +1893,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF6A8A8"/>
+      <color rgb="FFE583D9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2080,467 +2196,487 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" customWidth="1"/>
     <col min="5" max="6" width="9.140625" hidden="1" customWidth="1"/>
     <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B2" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="120"/>
+      <c r="B2" s="85" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="60"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="95"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="9" t="s">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B7" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="102"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="2:6" ht="30.75" thickBot="1">
-      <c r="B7" s="13" t="s">
+    </row>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B11" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="130" t="s">
+      <c r="C11" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="127"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B11" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="14" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B14" s="129" t="s">
+      <c r="B14" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="60"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="95"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="142" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="88" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="142" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="146" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="142" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="146" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B20" s="143" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="147" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B21" s="107" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="108"/>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B22" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B23" s="144" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="90" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B24" s="144" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="120"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="126" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="127"/>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="30">
-      <c r="B17" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="30">
-      <c r="B19" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="30">
-      <c r="B20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="128" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="122"/>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B22" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B23" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B24" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B25" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B26" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>50</v>
+      <c r="B25" s="144" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="91" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B26" s="145" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="93" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="28" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="29" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B29" s="119" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="120"/>
+      <c r="B29" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="110"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B30" s="121" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="122"/>
+      <c r="B30" s="141" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="59"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" customHeight="1">
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
+      <c r="B32" s="137" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="138" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>9</v>
+      <c r="B33" s="139" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="140" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="123" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="122"/>
+      <c r="B34" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="86"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B35" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>4</v>
+      <c r="B35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="136" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B37" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="86"/>
+    </row>
+    <row r="38" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="20" t="s">
+    </row>
+    <row r="39" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B39" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B37" s="124" t="s">
+      <c r="C39" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="30" customHeight="1">
+      <c r="B40" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="122"/>
-    </row>
-    <row r="38" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B38" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B39" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="30" customHeight="1">
-      <c r="B40" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>31</v>
+      <c r="C40" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B41" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>40</v>
+      <c r="B41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="43" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B44" s="125" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="120"/>
+      <c r="B44" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" s="80"/>
     </row>
     <row r="45" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B45" s="109" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="110"/>
+      <c r="B45" s="111" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="129"/>
     </row>
     <row r="46" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B46" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="52" t="s">
-        <v>4</v>
+      <c r="B46" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="113" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B47" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="54" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B48" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" s="40" customFormat="1" ht="30" customHeight="1">
-      <c r="B49" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" s="56" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B50" s="74" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B51" s="111" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="112"/>
+      <c r="B47" s="131" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="132" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B48" s="130" t="s">
+        <v>149</v>
+      </c>
+      <c r="C48" s="133" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" s="15" customFormat="1" ht="30" customHeight="1">
+      <c r="B49" s="130" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="133" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B50" s="130" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="114" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B51" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" s="116" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="52" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B52" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B53" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="C53" s="61" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B54" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="C54" s="61" t="s">
-        <v>86</v>
+      <c r="B52" s="117" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="118"/>
+    </row>
+    <row r="53" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B53" s="119" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B54" s="121" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="122" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B55" s="113" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" s="114"/>
-    </row>
-    <row r="56" spans="2:3" ht="30" customHeight="1">
-      <c r="B56" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" s="63" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B57" s="65" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="64" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="59" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="60" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B60" s="115" t="s">
-        <v>92</v>
-      </c>
-      <c r="C60" s="116"/>
-    </row>
-    <row r="61" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B61" s="117" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="118"/>
-    </row>
-    <row r="62" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B62" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="67" t="s">
-        <v>4</v>
-      </c>
+      <c r="B55" s="154" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="155"/>
+    </row>
+    <row r="56" spans="2:3" ht="15" customHeight="1">
+      <c r="B56" s="152" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B57" s="156" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="157" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B58" s="156" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="157" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B59" s="158" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" s="159" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" ht="12" customHeight="1">
+      <c r="B60" s="58"/>
+      <c r="C60" s="58"/>
+    </row>
+    <row r="61" spans="2:3" ht="21" customHeight="1">
+      <c r="B61" s="58"/>
+      <c r="C61" s="58"/>
+    </row>
+    <row r="62" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B62" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="62"/>
     </row>
     <row r="63" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B63" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="69" t="s">
-        <v>94</v>
-      </c>
+      <c r="B63" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="84"/>
     </row>
     <row r="64" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B64" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="69" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B65" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" s="108"/>
-    </row>
-    <row r="66" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B66" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B67" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="73" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="69" spans="2:3" ht="15.75" customHeight="1"/>
+      <c r="B64" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B65" s="125" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65" s="126" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B66" s="148" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" s="149" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B67" s="150" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" s="151"/>
+    </row>
+    <row r="68" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B68" s="152" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B69" s="127" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="128" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="70" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="71" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="72" spans="2:3" ht="15.75" customHeight="1"/>
@@ -3476,23 +3612,23 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3501,10 +3637,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M999"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:S999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3515,342 +3665,425 @@
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="13" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="35.140625" customWidth="1"/>
+    <col min="15" max="15" width="58.42578125" customWidth="1"/>
+    <col min="16" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="145" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="131" t="s">
+    <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1">
+      <c r="B2" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="M2" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2" s="160" t="s">
+        <v>182</v>
+      </c>
+      <c r="O2" s="160" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="78"/>
+      <c r="F3" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="52">
+        <v>0</v>
+      </c>
+      <c r="N3" s="161" t="s">
+        <v>184</v>
+      </c>
+      <c r="O3" s="161" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" customHeight="1">
+      <c r="A4" s="71"/>
+      <c r="B4" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="76"/>
+      <c r="M4" s="52">
+        <v>1</v>
+      </c>
+      <c r="N4" s="161" t="s">
+        <v>185</v>
+      </c>
+      <c r="O4" s="161" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1">
+      <c r="A5" s="20">
+        <v>0</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="52">
+        <v>2</v>
+      </c>
+      <c r="N5" s="161" t="s">
+        <v>186</v>
+      </c>
+      <c r="O5" s="161" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="30" customHeight="1">
+      <c r="A6" s="20">
+        <v>1</v>
+      </c>
+      <c r="B6" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="52">
+        <v>3</v>
+      </c>
+      <c r="N6" s="161" t="s">
+        <v>187</v>
+      </c>
+      <c r="O6" s="161" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1">
+      <c r="A7" s="20">
+        <v>2</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="52"/>
+      <c r="N7" s="161" t="s">
+        <v>188</v>
+      </c>
+      <c r="O7" s="161" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="26" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A8" s="20">
+        <v>3</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="74"/>
+      <c r="E8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="52">
+        <v>5</v>
+      </c>
+      <c r="N8" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="O8" s="161" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="45" customHeight="1">
+      <c r="A9" s="20">
+        <v>4</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="52">
+        <v>6</v>
+      </c>
+      <c r="N9" s="161" t="s">
+        <v>191</v>
+      </c>
+      <c r="O9" s="161" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="30" customHeight="1">
+      <c r="A10" s="20">
+        <v>5</v>
+      </c>
+      <c r="B10" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="161" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="30" customHeight="1">
+      <c r="A11" s="20">
+        <v>6</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="65"/>
+      <c r="D11" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="65"/>
+      <c r="F11" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1">
+      <c r="A12" s="20">
+        <v>7</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1" thickBot="1">
+      <c r="A13" s="24">
+        <v>8</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="133" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="133"/>
-      <c r="D3" s="133" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="133"/>
-      <c r="F3" s="134" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="132"/>
-      <c r="B4" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="135"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="45">
+    </row>
+    <row r="14" spans="1:19" ht="15" customHeight="1">
+      <c r="S14" s="42" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" customHeight="1" thickBot="1">
+      <c r="A16" s="26"/>
+      <c r="B16" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="26"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1">
+      <c r="A17" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="78"/>
+      <c r="F17" s="75" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1">
+      <c r="A18" s="71"/>
+      <c r="B18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="76"/>
+    </row>
+    <row r="19" spans="1:13" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="20">
         <v>0</v>
       </c>
-      <c r="B5" s="142" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="143"/>
-      <c r="D5" s="143"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="A6" s="45">
+      <c r="B19" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="142" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="144"/>
-      <c r="F6" s="47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="45">
+      <c r="B20" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A21" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="142" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="47" t="s">
+      <c r="B21" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="45" customHeight="1">
+      <c r="A22" s="20">
+        <v>3</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="74"/>
+      <c r="E22" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" customHeight="1">
+      <c r="A23" s="20">
+        <v>4</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="64"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" customHeight="1">
+      <c r="A24" s="20">
+        <v>5</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="75" customFormat="1" ht="84.75" customHeight="1">
-      <c r="A8" s="45">
-        <v>3</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="142" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="144"/>
-      <c r="E8" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" customHeight="1">
-      <c r="A9" s="45">
-        <v>4</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="136" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="137"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="47" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
-      <c r="A10" s="45">
-        <v>5</v>
-      </c>
-      <c r="B10" s="136" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="137"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
-      <c r="A11" s="45">
+      <c r="M24" s="42"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A25" s="20">
         <v>6</v>
       </c>
-      <c r="B11" s="136" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="138"/>
-      <c r="D11" s="146" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="138"/>
-      <c r="F11" s="48" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="45">
+      <c r="B25" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A26" s="24">
         <v>7</v>
       </c>
-      <c r="B12" s="136" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="137"/>
-      <c r="D12" s="137"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="49">
-        <v>8</v>
-      </c>
-      <c r="B13" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="50" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A16" s="75"/>
-      <c r="B16" s="145" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" s="145"/>
-      <c r="D16" s="145"/>
-      <c r="E16" s="145"/>
-      <c r="F16" s="75"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1">
-      <c r="A17" s="131" t="s">
+      <c r="B26" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="25" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" s="133" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="133"/>
-      <c r="D17" s="133" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="133"/>
-      <c r="F17" s="134" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="132"/>
-      <c r="B18" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="135"/>
-    </row>
-    <row r="19" spans="1:13" s="44" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="45">
-        <v>0</v>
-      </c>
-      <c r="B19" s="142" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="143"/>
-      <c r="D19" s="143"/>
-      <c r="E19" s="144"/>
-      <c r="F19" s="46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="45">
-        <v>1</v>
-      </c>
-      <c r="B20" s="142" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="143"/>
-      <c r="D20" s="143"/>
-      <c r="E20" s="144"/>
-      <c r="F20" s="47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="45">
-        <v>2</v>
-      </c>
-      <c r="B21" s="142" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="143"/>
-      <c r="D21" s="143"/>
-      <c r="E21" s="144"/>
-      <c r="F21" s="48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="45" customHeight="1">
-      <c r="A22" s="45">
-        <v>3</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="142" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="144"/>
-      <c r="E22" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="47" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="30" customHeight="1">
-      <c r="A23" s="45">
-        <v>4</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="136" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="90" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="30" customHeight="1">
-      <c r="A24" s="45">
-        <v>5</v>
-      </c>
-      <c r="B24" s="136" t="s">
-        <v>119</v>
-      </c>
-      <c r="C24" s="137"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="M24" s="91"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="45">
-        <v>6</v>
-      </c>
-      <c r="B25" s="136" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="137"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="49">
-        <v>7</v>
-      </c>
-      <c r="B26" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="141"/>
-      <c r="F26" s="50" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1"/>
@@ -4828,6 +5061,26 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B10:E10"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B16:E16"/>
@@ -4836,38 +5089,18 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4878,160 +5111,160 @@
   <sheetData>
     <row r="2" spans="2:3" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:3">
-      <c r="B3" s="76" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>105</v>
+      <c r="B3" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="30.75" thickBot="1">
-      <c r="B4" s="87" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="88">
+      <c r="B4" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="39">
         <v>43579</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B5" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="86" t="s">
-        <v>109</v>
+      <c r="B5" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="83" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="84" t="s">
-        <v>127</v>
+      <c r="B6" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="78" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="80" t="s">
-        <v>127</v>
+      <c r="B7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="78" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="80" t="s">
-        <v>127</v>
+      <c r="B8" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="80" t="s">
-        <v>127</v>
+      <c r="B9" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>127</v>
+      <c r="B10" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="80" t="s">
-        <v>127</v>
+      <c r="B11" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="79"/>
-      <c r="C12" s="80"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="79"/>
-      <c r="C13" s="80"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="79"/>
-      <c r="C14" s="80"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="79"/>
-      <c r="C15" s="80"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="79"/>
-      <c r="C16" s="80"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="79"/>
-      <c r="C17" s="80"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="79"/>
-      <c r="C19" s="80"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="79"/>
-      <c r="C20" s="80"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
     </row>
     <row r="21" spans="2:3">
-      <c r="B21" s="79"/>
-      <c r="C21" s="80"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="2:3">
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
     </row>
     <row r="23" spans="2:3">
-      <c r="B23" s="79"/>
-      <c r="C23" s="80"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="2:3">
-      <c r="B24" s="79"/>
-      <c r="C24" s="80"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="79"/>
-      <c r="C25" s="80"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="79"/>
-      <c r="C26" s="80"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="79"/>
-      <c r="C27" s="80"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="79"/>
-      <c r="C28" s="80"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="29" spans="2:3">
-      <c r="B29" s="79"/>
-      <c r="C29" s="80"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="79"/>
-      <c r="C30" s="80"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="79"/>
-      <c r="C31" s="80"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
     </row>
     <row r="32" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B32" s="81"/>
-      <c r="C32" s="82"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5039,12 +5272,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5058,519 +5291,519 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="19.5" thickBot="1">
-      <c r="B2" s="147" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="G2" s="149" t="s">
-        <v>167</v>
-      </c>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
+      <c r="B2" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="G2" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="98" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="99" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="100" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="98" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="99" t="s">
-        <v>130</v>
-      </c>
-      <c r="I3" s="100" t="s">
-        <v>129</v>
+      <c r="B3" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="45">
+      <c r="B4" s="20">
         <v>0</v>
       </c>
-      <c r="C4" s="92" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="93" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="104">
+      <c r="C4" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="55">
         <v>0</v>
       </c>
-      <c r="H4" s="105">
+      <c r="H4" s="56">
         <v>0</v>
       </c>
-      <c r="I4" s="106" t="s">
-        <v>153</v>
+      <c r="I4" s="57" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="2:9">
-      <c r="B5" s="45">
+      <c r="B5" s="20">
         <v>1</v>
       </c>
-      <c r="C5" s="92" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="93" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="45">
+      <c r="C5" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="20">
         <v>1</v>
       </c>
-      <c r="H5" s="94">
+      <c r="H5" s="45">
         <v>0</v>
       </c>
-      <c r="I5" s="93" t="s">
-        <v>154</v>
+      <c r="I5" s="44" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30">
-      <c r="B6" s="45">
+      <c r="B6" s="20">
         <v>2</v>
       </c>
-      <c r="C6" s="92" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="93" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="45">
+      <c r="C6" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="20">
         <v>2</v>
       </c>
-      <c r="H6" s="92" t="s">
-        <v>170</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>169</v>
+      <c r="H6" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:9">
-      <c r="B7" s="45">
+      <c r="B7" s="20">
         <v>3</v>
       </c>
-      <c r="C7" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="93" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="45">
+      <c r="C7" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="20">
         <v>3</v>
       </c>
-      <c r="H7" s="94"/>
-      <c r="I7" s="95" t="s">
-        <v>147</v>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="45">
+      <c r="B8" s="20">
         <v>4</v>
       </c>
-      <c r="C8" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="93" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="45">
+      <c r="C8" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="20">
         <v>4</v>
       </c>
-      <c r="H8" s="94"/>
-      <c r="I8" s="95" t="s">
-        <v>147</v>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="45">
+      <c r="B9" s="20">
         <v>5</v>
       </c>
-      <c r="C9" s="94">
+      <c r="C9" s="45">
         <v>0</v>
       </c>
-      <c r="D9" s="95" t="s">
-        <v>145</v>
-      </c>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="45">
+      <c r="D9" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="20">
         <v>5</v>
       </c>
-      <c r="H9" s="94">
+      <c r="H9" s="45">
         <v>0</v>
       </c>
-      <c r="I9" s="95" t="s">
-        <v>145</v>
+      <c r="I9" s="46" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="45">
+      <c r="B10" s="20">
         <v>6</v>
       </c>
-      <c r="C10" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="95" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="45">
+      <c r="C10" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="20">
         <v>6</v>
       </c>
-      <c r="H10" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="I10" s="95" t="s">
-        <v>146</v>
+      <c r="H10" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="45">
+      <c r="B11" s="20">
         <v>7</v>
       </c>
-      <c r="C11" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="D11" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="45">
+      <c r="C11" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="20">
         <v>7</v>
       </c>
-      <c r="H11" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="I11" s="95" t="s">
-        <v>155</v>
+      <c r="H11" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="45">
+      <c r="B12" s="20">
         <v>8</v>
       </c>
-      <c r="C12" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="D12" s="93" t="s">
-        <v>165</v>
-      </c>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="45">
+      <c r="C12" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="20">
         <v>8</v>
       </c>
-      <c r="H12" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="I12" s="95" t="s">
-        <v>156</v>
+      <c r="H12" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="45">
+      <c r="B13" s="20">
         <v>9</v>
       </c>
-      <c r="C13" s="92" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" s="93" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="45">
+      <c r="C13" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="20">
         <v>9</v>
       </c>
-      <c r="H13" s="94"/>
-      <c r="I13" s="95" t="s">
-        <v>147</v>
+      <c r="H13" s="45"/>
+      <c r="I13" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="45">
+      <c r="B14" s="20">
         <v>10</v>
       </c>
-      <c r="C14" s="92" t="s">
-        <v>139</v>
-      </c>
-      <c r="D14" s="93" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="45">
+      <c r="C14" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="20">
         <v>10</v>
       </c>
-      <c r="H14" s="94"/>
-      <c r="I14" s="95" t="s">
-        <v>147</v>
+      <c r="H14" s="45"/>
+      <c r="I14" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="45">
+      <c r="B15" s="20">
         <v>11</v>
       </c>
-      <c r="C15" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="95" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="45">
+      <c r="C15" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="20">
         <v>11</v>
       </c>
-      <c r="H15" s="94"/>
-      <c r="I15" s="95" t="s">
-        <v>147</v>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="45">
+      <c r="B16" s="20">
         <v>12</v>
       </c>
-      <c r="C16" s="92" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" s="93" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="45">
+      <c r="C16" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="20">
         <v>12</v>
       </c>
-      <c r="H16" s="92" t="s">
-        <v>162</v>
-      </c>
-      <c r="I16" s="93" t="s">
-        <v>163</v>
+      <c r="H16" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="44" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="30">
-      <c r="B17" s="45">
+      <c r="B17" s="20">
         <v>13</v>
       </c>
-      <c r="C17" s="92" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="45">
+      <c r="C17" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="20">
         <v>13</v>
       </c>
-      <c r="H17" s="94"/>
-      <c r="I17" s="95" t="s">
-        <v>147</v>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="30">
-      <c r="B18" s="45">
+      <c r="B18" s="20">
         <v>14</v>
       </c>
-      <c r="C18" s="92" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="45">
+      <c r="C18" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="20">
         <v>14</v>
       </c>
-      <c r="H18" s="94"/>
-      <c r="I18" s="95" t="s">
-        <v>147</v>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="45">
+      <c r="B19" s="20">
         <v>15</v>
       </c>
-      <c r="C19" s="103"/>
-      <c r="D19" s="93" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="45">
+      <c r="C19" s="54"/>
+      <c r="D19" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="20">
         <v>15</v>
       </c>
-      <c r="H19" s="94"/>
-      <c r="I19" s="95" t="s">
-        <v>147</v>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="45">
+      <c r="B20" s="20">
         <v>16</v>
       </c>
-      <c r="C20" s="94"/>
-      <c r="D20" s="93" t="s">
-        <v>142</v>
-      </c>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="45">
+      <c r="C20" s="45"/>
+      <c r="D20" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="20">
         <v>16</v>
       </c>
-      <c r="H20" s="94"/>
-      <c r="I20" s="95" t="s">
-        <v>147</v>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="B21" s="45">
+      <c r="B21" s="20">
         <v>17</v>
       </c>
-      <c r="C21" s="92"/>
-      <c r="D21" s="93" t="s">
-        <v>141</v>
-      </c>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="45">
+      <c r="C21" s="43"/>
+      <c r="D21" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="20">
         <v>17</v>
       </c>
-      <c r="H21" s="94"/>
-      <c r="I21" s="95" t="s">
-        <v>147</v>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="45">
+      <c r="B22" s="20">
         <v>18</v>
       </c>
-      <c r="C22" s="94" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22" s="95" t="s">
-        <v>152</v>
-      </c>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="45">
+      <c r="C22" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="20">
         <v>18</v>
       </c>
-      <c r="H22" s="94" t="s">
-        <v>132</v>
-      </c>
-      <c r="I22" s="95" t="s">
-        <v>152</v>
+      <c r="H22" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="46" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="45">
+      <c r="B23" s="20">
         <v>19</v>
       </c>
-      <c r="C23" s="94" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="45">
+      <c r="C23" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="20">
         <v>19</v>
       </c>
-      <c r="H23" s="94" t="s">
-        <v>131</v>
-      </c>
-      <c r="I23" s="95" t="s">
-        <v>151</v>
+      <c r="H23" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" s="46" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="45">
+      <c r="B24" s="20">
         <v>20</v>
       </c>
-      <c r="C24" s="94" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="93" t="s">
-        <v>149</v>
-      </c>
-      <c r="E24" s="89"/>
-      <c r="F24" s="89"/>
-      <c r="G24" s="45">
+      <c r="C24" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="20">
         <v>20</v>
       </c>
-      <c r="H24" s="94" t="s">
-        <v>133</v>
-      </c>
-      <c r="I24" s="93" t="s">
-        <v>149</v>
+      <c r="H24" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="44" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B25" s="49">
+      <c r="B25" s="24">
         <v>21</v>
       </c>
-      <c r="C25" s="96">
+      <c r="C25" s="47">
         <v>0</v>
       </c>
-      <c r="D25" s="97" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="49">
+      <c r="D25" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="24">
         <v>21</v>
       </c>
-      <c r="H25" s="96">
+      <c r="H25" s="47">
         <v>0</v>
       </c>
-      <c r="I25" s="97" t="s">
-        <v>150</v>
+      <c r="I25" s="48" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:9">
-      <c r="B26" s="102"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
+      <c r="B26" s="53"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
     </row>
     <row r="27" spans="2:9">
-      <c r="B27" s="102"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="101"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
     </row>
     <row r="28" spans="2:9">
-      <c r="B28" s="102"/>
-      <c r="C28" s="102"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="101"/>
-      <c r="I28" s="101"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
     </row>
   </sheetData>
   <sortState ref="B4:G27">

</xml_diff>

<commit_message>
SCROD and DC Register Programming successful, QBLink Ping Test successful
</commit_message>
<xml_diff>
--- a/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
+++ b/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34ABC965-A242-46AF-8020-27CD15DF7F89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="2"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23028" windowHeight="12948" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD side Signals" sheetId="1" r:id="rId1"/>
@@ -14,12 +20,11 @@
     <sheet name="Register" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="201">
   <si>
     <t>From PC/Input Signals</t>
   </si>
@@ -307,9 +312,6 @@
   </si>
   <si>
     <t>mppc dac voltage</t>
-  </si>
-  <si>
-    <t>mppc dac address on TargetX</t>
   </si>
   <si>
     <t>0, 4</t>
@@ -394,9 +396,6 @@
     <t>15, 1 downto 0</t>
   </si>
   <si>
-    <t>sets wait period for digitizing ramp</t>
-  </si>
-  <si>
     <t>15, 8 downto 0</t>
   </si>
   <si>
@@ -415,9 +414,6 @@
     <t>SCROD FPGA Control Registers</t>
   </si>
   <si>
-    <t xml:space="preserve">Device labels: (SCROD) 0x00A5,            (DC) 0x00DC | Device  #: 0x00 (SCROD), 0x01 through 0x08 (DC #) or 0x0A for broadcasting to all DCs. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sync Daughtercards, reset QBLink (*msb depends on how many DC you have) </t>
   </si>
   <si>
@@ -623,12 +619,85 @@
   </si>
   <si>
     <t>checksum</t>
+  </si>
+  <si>
+    <t>mppc dac address on TargetX (PCLK #)</t>
+  </si>
+  <si>
+    <t>mppc dac voltage (12-bit code)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Device labels:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (SCROD) 0x00A5, (DC) 0x00DC   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Device  #:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  (SCROD) 0x00 , (DCs) DC# or 0x0A for broadcasting to all DCs. </t>
+    </r>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Number of remaining words except packet checksum</t>
+  </si>
+  <si>
+    <t>(sending one command has 6 operations) 0x00000006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Target device is SCROD) 0x0000A500 (Broadcast to all DCs) 0x0000DC0A           </t>
+  </si>
+  <si>
+    <t>Verb(7): suppresses command response, Verb(others) = '0'. Command ID: unique ID to each command</t>
+  </si>
+  <si>
+    <t>(no verbosity) 0x00000012</t>
+  </si>
+  <si>
+    <t>(write) 0x72697465</t>
+  </si>
+  <si>
+    <t>(write value 1 to register 1) 0x00010001</t>
+  </si>
+  <si>
+    <t>0x726A7478</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -810,7 +879,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1442,11 +1511,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1573,7 +1651,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1586,12 +1663,303 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1628,263 +1996,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1902,6 +2041,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1950,7 +2092,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1983,9 +2125,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2018,6 +2177,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2193,217 +2369,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F1002"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="32.41796875" customWidth="1"/>
+    <col min="3" max="3" width="46.15625" customWidth="1"/>
+    <col min="4" max="4" width="31.83984375" customWidth="1"/>
+    <col min="5" max="6" width="9.15625" hidden="1" customWidth="1"/>
+    <col min="7" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B2" s="85" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="60"/>
+    <row r="2" spans="2:6" ht="18.600000000000001" thickBot="1">
+      <c r="B2" s="136" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="137"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="94" t="s">
+    <row r="3" spans="2:6" ht="14.4">
+      <c r="B3" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="95"/>
+      <c r="C3" s="133"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="96" t="s">
+    <row r="4" spans="2:6" ht="14.4">
+      <c r="B4" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="66" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="87" t="s">
+    <row r="5" spans="2:6" ht="14.4">
+      <c r="B5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="67" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="87" t="s">
+    <row r="6" spans="2:6" ht="14.4">
+      <c r="B6" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="59" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B7" s="99" t="s">
+    <row r="7" spans="2:6" ht="14.7" thickBot="1">
+      <c r="B7" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="69" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="101" t="s">
+    <row r="8" spans="2:6" ht="14.4">
+      <c r="B8" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="102"/>
+      <c r="C8" s="139"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="103" t="s">
+    <row r="9" spans="2:6" ht="14.4">
+      <c r="B9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="104" t="s">
+      <c r="C9" s="71" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="89" t="s">
+    <row r="10" spans="2:6" ht="14.4">
+      <c r="B10" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="72" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B11" s="92" t="s">
+    <row r="11" spans="2:6" ht="14.7" thickBot="1">
+      <c r="B11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="73" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B14" s="85" t="s">
+    <row r="14" spans="2:6" ht="18.600000000000001" thickBot="1">
+      <c r="B14" s="136" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="137"/>
+    </row>
+    <row r="15" spans="2:6" ht="14.4">
+      <c r="B15" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="133"/>
+    </row>
+    <row r="16" spans="2:6" ht="14.4">
+      <c r="B16" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="14.4">
+      <c r="B17" s="98" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="14.4">
+      <c r="B18" s="98" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="102" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="14.4">
+      <c r="B19" s="98" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" s="102" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="14.7" thickBot="1">
+      <c r="B20" s="99" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="103" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B21" s="134" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="60"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="94" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="95"/>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="96" t="s">
+      <c r="C21" s="135"/>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B22" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="97" t="s">
+      <c r="C22" s="71" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="142" t="s">
-        <v>172</v>
-      </c>
-      <c r="C17" s="88" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="142" t="s">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B23" s="100" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="146" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="142" t="s">
+      <c r="C23" s="61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B24" s="100" t="s">
         <v>163</v>
       </c>
-      <c r="C19" s="146" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B20" s="143" t="s">
+      <c r="C24" s="62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B25" s="100" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="147" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="107" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21" s="108"/>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B22" s="103" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="104" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B23" s="144" t="s">
+      <c r="C25" s="62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B26" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="C23" s="90" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B24" s="144" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" s="91" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B25" s="144" t="s">
-        <v>167</v>
-      </c>
-      <c r="C25" s="91" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B26" s="145" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="93" t="s">
+      <c r="C26" s="64" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="28" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="29" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B29" s="109" t="s">
+      <c r="B29" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="110"/>
+      <c r="C29" s="141"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B30" s="141" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="59"/>
+      <c r="B30" s="142" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="143"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" customHeight="1">
       <c r="B31" s="2" t="s">
@@ -2414,26 +2590,26 @@
       </c>
     </row>
     <row r="32" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B32" s="137" t="s">
-        <v>156</v>
-      </c>
-      <c r="C32" s="138" t="s">
-        <v>161</v>
+      <c r="B32" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="95" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B33" s="139" t="s">
+      <c r="B33" s="96" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="97" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B34" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="C33" s="140" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="134" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" s="86"/>
+      <c r="C34" s="145"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="6" t="s">
@@ -2444,18 +2620,18 @@
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="136" t="s">
-        <v>155</v>
+      <c r="B36" s="93" t="s">
+        <v>152</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B37" s="135" t="s">
+      <c r="B37" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="86"/>
+      <c r="C37" s="145"/>
     </row>
     <row r="38" spans="2:3" ht="15.75" customHeight="1">
       <c r="B38" s="9" t="s">
@@ -2492,189 +2668,189 @@
     <row r="42" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="43" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B44" s="79" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="80"/>
+      <c r="B44" s="147" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="148"/>
     </row>
     <row r="45" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B45" s="111" t="s">
+      <c r="B45" s="151" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="129"/>
+      <c r="C45" s="152"/>
     </row>
     <row r="46" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B46" s="112" t="s">
+      <c r="B46" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="113" t="s">
+      <c r="C46" s="75" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B47" s="131" t="s">
+      <c r="B47" s="90" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="91" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B48" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="92" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" s="15" customFormat="1" ht="30" customHeight="1">
+      <c r="B49" s="89" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="C47" s="132" t="s">
+    </row>
+    <row r="50" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B50" s="89" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B51" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="78" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B52" s="153" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="154"/>
+    </row>
+    <row r="53" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B53" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B54" s="81" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="82" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B55" s="155" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="156"/>
+    </row>
+    <row r="56" spans="2:3" ht="15" customHeight="1">
+      <c r="B56" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B57" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="109" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B58" s="108" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="109" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B59" s="110" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="111" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B48" s="130" t="s">
-        <v>149</v>
-      </c>
-      <c r="C48" s="133" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" s="15" customFormat="1" ht="30" customHeight="1">
-      <c r="B49" s="130" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" s="133" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B50" s="130" t="s">
-        <v>146</v>
-      </c>
-      <c r="C50" s="114" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B51" s="115" t="s">
-        <v>147</v>
-      </c>
-      <c r="C51" s="116" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B52" s="117" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="118"/>
-    </row>
-    <row r="53" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B53" s="119" t="s">
+    <row r="60" spans="2:3" ht="12" customHeight="1">
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+    </row>
+    <row r="61" spans="2:3" ht="21" customHeight="1">
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+    </row>
+    <row r="62" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B62" s="157" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="158"/>
+    </row>
+    <row r="63" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B63" s="159" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="160"/>
+    </row>
+    <row r="64" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B64" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="120" t="s">
+      <c r="C64" s="84" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B54" s="121" t="s">
+    <row r="65" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B65" s="85" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="86" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B66" s="104" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="105" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B67" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" s="150"/>
+    </row>
+    <row r="68" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B68" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B69" s="87" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="122" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B55" s="154" t="s">
-        <v>135</v>
-      </c>
-      <c r="C55" s="155"/>
-    </row>
-    <row r="56" spans="2:3" ht="15" customHeight="1">
-      <c r="B56" s="152" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="153" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B57" s="156" t="s">
-        <v>139</v>
-      </c>
-      <c r="C57" s="157" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B58" s="156" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="157" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B59" s="158" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" s="159" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" ht="12" customHeight="1">
-      <c r="B60" s="58"/>
-      <c r="C60" s="58"/>
-    </row>
-    <row r="61" spans="2:3" ht="21" customHeight="1">
-      <c r="B61" s="58"/>
-      <c r="C61" s="58"/>
-    </row>
-    <row r="62" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B62" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="C62" s="62"/>
-    </row>
-    <row r="63" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B63" s="83" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="84"/>
-    </row>
-    <row r="64" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B64" s="123" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="124" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B65" s="125" t="s">
-        <v>142</v>
-      </c>
-      <c r="C65" s="126" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B66" s="148" t="s">
+      <c r="C69" s="88" t="s">
         <v>141</v>
-      </c>
-      <c r="C66" s="149" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B67" s="150" t="s">
-        <v>57</v>
-      </c>
-      <c r="C67" s="151"/>
-    </row>
-    <row r="68" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B68" s="152" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="153" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B69" s="127" t="s">
-        <v>143</v>
-      </c>
-      <c r="C69" s="128" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="15.75" customHeight="1"/>
@@ -3636,85 +3812,90 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S999"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:T999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" customWidth="1"/>
-    <col min="7" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="35.140625" customWidth="1"/>
-    <col min="15" max="15" width="58.42578125" customWidth="1"/>
-    <col min="16" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="16.41796875" customWidth="1"/>
+    <col min="3" max="3" width="16.15625" customWidth="1"/>
+    <col min="4" max="4" width="13.15625" customWidth="1"/>
+    <col min="5" max="5" width="16.26171875" customWidth="1"/>
+    <col min="6" max="6" width="37.15625" style="115" customWidth="1"/>
+    <col min="7" max="7" width="37.41796875" customWidth="1"/>
+    <col min="8" max="14" width="8.68359375" customWidth="1"/>
+    <col min="15" max="15" width="35.15625" customWidth="1"/>
+    <col min="16" max="16" width="58.41796875" customWidth="1"/>
+    <col min="17" max="27" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="69" t="s">
+    <row r="2" spans="1:20" ht="15" customHeight="1" thickBot="1">
+      <c r="B2" s="167" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="M2" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="N2" s="160" t="s">
-        <v>182</v>
-      </c>
-      <c r="O2" s="160" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="70" t="s">
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="114"/>
+      <c r="N2" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="P2" s="112" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1">
+      <c r="A3" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="176" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78" t="s">
+      <c r="C3" s="176"/>
+      <c r="D3" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="75" t="s">
+      <c r="E3" s="176"/>
+      <c r="F3" s="177" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="52">
+      <c r="G3" s="173" t="s">
+        <v>192</v>
+      </c>
+      <c r="N3" s="52">
         <v>0</v>
       </c>
-      <c r="N3" s="161" t="s">
-        <v>184</v>
-      </c>
-      <c r="O3" s="161" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1">
-      <c r="A4" s="71"/>
+      <c r="O3" s="113" t="s">
+        <v>181</v>
+      </c>
+      <c r="P3" s="113" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1">
+      <c r="A4" s="169"/>
       <c r="B4" s="16" t="s">
         <v>33</v>
       </c>
@@ -3727,232 +3908,260 @@
       <c r="E4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="M4" s="52">
+      <c r="F4" s="178"/>
+      <c r="G4" s="174"/>
+      <c r="N4" s="52">
         <v>1</v>
       </c>
-      <c r="N4" s="161" t="s">
-        <v>185</v>
-      </c>
-      <c r="O4" s="161" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1">
+      <c r="O4" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="P4" s="113" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1">
       <c r="A5" s="20">
         <v>0</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="21" t="s">
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="52">
+      <c r="G5" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="52">
         <v>2</v>
       </c>
-      <c r="N5" s="161" t="s">
-        <v>186</v>
-      </c>
-      <c r="O5" s="161" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="30" customHeight="1">
+      <c r="O5" s="113" t="s">
+        <v>183</v>
+      </c>
+      <c r="P5" s="113" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="30" customHeight="1">
       <c r="A6" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="M6" s="52">
+      <c r="C6" s="171"/>
+      <c r="D6" s="171"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" s="116" t="s">
+        <v>194</v>
+      </c>
+      <c r="N6" s="52">
         <v>3</v>
       </c>
-      <c r="N6" s="161" t="s">
-        <v>187</v>
-      </c>
-      <c r="O6" s="161" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1">
+      <c r="O6" s="113" t="s">
+        <v>184</v>
+      </c>
+      <c r="P6" s="113" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15" customHeight="1">
       <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="22" t="s">
+      <c r="C7" s="171"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="161" t="s">
-        <v>188</v>
-      </c>
-      <c r="O7" s="161" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="26" customFormat="1" ht="84.75" customHeight="1">
+      <c r="G7" s="129" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="52"/>
+      <c r="O7" s="113" t="s">
+        <v>185</v>
+      </c>
+      <c r="P7" s="113" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="26" customFormat="1" ht="84.75" customHeight="1">
       <c r="A8" s="20">
         <v>3</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="74"/>
+      <c r="D8" s="172"/>
       <c r="E8" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="M8" s="52">
+      <c r="F8" s="121" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="131" t="s">
+        <v>195</v>
+      </c>
+      <c r="N8" s="52">
         <v>5</v>
       </c>
-      <c r="N8" s="52" t="s">
-        <v>189</v>
-      </c>
-      <c r="O8" s="161" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="45" customHeight="1">
+      <c r="O8" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="P8" s="113" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="45" customHeight="1">
       <c r="A9" s="20">
         <v>4</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="161" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="52">
+      <c r="D9" s="162"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="123" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="130" t="s">
+        <v>197</v>
+      </c>
+      <c r="N9" s="52">
         <v>6</v>
       </c>
-      <c r="N9" s="161" t="s">
-        <v>191</v>
-      </c>
-      <c r="O9" s="161" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="30" customHeight="1">
+      <c r="O9" s="113" t="s">
+        <v>188</v>
+      </c>
+      <c r="P9" s="113" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="30" customHeight="1">
       <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="23" t="s">
+      <c r="C10" s="162"/>
+      <c r="D10" s="162"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="121" t="s">
         <v>80</v>
       </c>
-      <c r="M10" s="52"/>
+      <c r="G10" s="130" t="s">
+        <v>198</v>
+      </c>
       <c r="N10" s="52"/>
-      <c r="O10" s="161" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="30" customHeight="1">
+      <c r="O10" s="52"/>
+      <c r="P10" s="113" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="30" customHeight="1">
       <c r="A11" s="20">
         <v>6</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="161" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="77" t="s">
+      <c r="C11" s="163"/>
+      <c r="D11" s="175" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="23" t="s">
+      <c r="E11" s="163"/>
+      <c r="F11" s="121" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1">
+      <c r="G11" s="130" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15" customHeight="1">
       <c r="A12" s="20">
         <v>7</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="23" t="s">
+      <c r="C12" s="162"/>
+      <c r="D12" s="162"/>
+      <c r="E12" s="163"/>
+      <c r="F12" s="121" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" thickBot="1">
+      <c r="G12" s="130" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15" customHeight="1" thickBot="1">
       <c r="A13" s="24">
         <v>8</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="25" t="s">
+      <c r="C13" s="165"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="125" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1">
-      <c r="S14" s="42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" thickBot="1">
+      <c r="G13" s="130"/>
+    </row>
+    <row r="14" spans="1:20" ht="15" customHeight="1">
+      <c r="T14" s="42" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="26"/>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1">
-      <c r="A17" s="70" t="s">
+      <c r="C16" s="167"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1">
+      <c r="A17" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="176" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78" t="s">
+      <c r="C17" s="176"/>
+      <c r="D17" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="78"/>
-      <c r="F17" s="75" t="s">
+      <c r="E17" s="176"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="179" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="71"/>
+    <row r="18" spans="1:14" ht="15" customHeight="1">
+      <c r="A18" s="169"/>
       <c r="B18" s="16" t="s">
         <v>33</v>
       </c>
@@ -3965,133 +4174,142 @@
       <c r="E18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="76"/>
-    </row>
-    <row r="19" spans="1:13" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="F18" s="127"/>
+      <c r="G18" s="180"/>
+    </row>
+    <row r="19" spans="1:14" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="20">
         <v>0</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="21" t="s">
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1">
+    <row r="20" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1">
       <c r="A20" s="20">
         <v>1</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="22" t="s">
+      <c r="C20" s="171"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="20">
         <v>2</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="23" t="s">
+      <c r="C21" s="171"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="172"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="45" customHeight="1">
+    <row r="22" spans="1:14" ht="45" customHeight="1">
       <c r="A22" s="20">
         <v>3</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="74"/>
+      <c r="D22" s="172"/>
       <c r="E22" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="123"/>
+      <c r="G22" s="22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="30" customHeight="1">
+    <row r="23" spans="1:14" ht="30" customHeight="1">
       <c r="A23" s="20">
         <v>4</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="161" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="41" t="s">
+      <c r="D23" s="162"/>
+      <c r="E23" s="163"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="30" customHeight="1">
+    <row r="24" spans="1:14" ht="30" customHeight="1">
       <c r="A24" s="20">
         <v>5</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="161" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="23" t="s">
+      <c r="C24" s="162"/>
+      <c r="D24" s="162"/>
+      <c r="E24" s="163"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="M24" s="42"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N24" s="42"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="20">
         <v>6</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="23" t="s">
+      <c r="C25" s="162"/>
+      <c r="D25" s="162"/>
+      <c r="E25" s="163"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A26" s="24">
         <v>7</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="25" t="s">
+      <c r="C26" s="165"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="126"/>
+      <c r="G26" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="33" ht="30" customHeight="1"/>
     <row r="34" ht="30" customHeight="1"/>
     <row r="35" ht="47.25" customHeight="1"/>
@@ -5060,11 +5278,11 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B26:E26"/>
@@ -5073,7 +5291,7 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B11:C11"/>
@@ -5081,6 +5299,7 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B16:E16"/>
@@ -5096,20 +5315,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.68359375" customWidth="1"/>
+    <col min="3" max="3" width="20.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:3" ht="14.7" thickBot="1"/>
     <row r="3" spans="2:3">
       <c r="B3" s="27" t="s">
         <v>60</v>
@@ -5118,7 +5337,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" thickBot="1">
+    <row r="4" spans="2:3" ht="29.1" thickBot="1">
       <c r="B4" s="38" t="s">
         <v>61</v>
       </c>
@@ -5126,7 +5345,7 @@
         <v>43579</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" thickBot="1">
+    <row r="5" spans="2:3" ht="14.7" thickBot="1">
       <c r="B5" s="36" t="s">
         <v>62</v>
       </c>
@@ -5262,7 +5481,7 @@
       <c r="B31" s="30"/>
       <c r="C31" s="31"/>
     </row>
-    <row r="32" spans="2:3" ht="15.75" thickBot="1">
+    <row r="32" spans="2:3" ht="14.7" thickBot="1">
       <c r="B32" s="32"/>
       <c r="C32" s="33"/>
     </row>
@@ -5273,34 +5492,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.15625" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.41796875" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="51.28515625" customWidth="1"/>
+    <col min="9" max="9" width="51.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="19.5" thickBot="1">
-      <c r="B2" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="G2" s="81" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+    <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1">
+      <c r="B2" s="147" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="G2" s="181" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" s="49" t="s">
@@ -5327,21 +5546,21 @@
         <v>0</v>
       </c>
       <c r="C4" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="44" t="s">
         <v>97</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>98</v>
       </c>
       <c r="E4" s="40"/>
       <c r="F4" s="40"/>
-      <c r="G4" s="55">
+      <c r="G4" s="54">
         <v>0</v>
       </c>
-      <c r="H4" s="56">
+      <c r="H4" s="55">
         <v>0</v>
       </c>
-      <c r="I4" s="57" t="s">
-        <v>107</v>
+      <c r="I4" s="56" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -5363,10 +5582,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="30">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="28.8">
       <c r="B6" s="20">
         <v>2</v>
       </c>
@@ -5382,10 +5601,10 @@
         <v>2</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -5405,7 +5624,7 @@
       </c>
       <c r="H7" s="45"/>
       <c r="I7" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -5425,7 +5644,7 @@
       </c>
       <c r="H8" s="45"/>
       <c r="I8" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -5436,7 +5655,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="40"/>
       <c r="F9" s="40"/>
@@ -5447,7 +5666,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -5458,7 +5677,7 @@
         <v>92</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
@@ -5469,7 +5688,7 @@
         <v>92</v>
       </c>
       <c r="I10" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -5480,7 +5699,7 @@
         <v>92</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
@@ -5491,7 +5710,7 @@
         <v>92</v>
       </c>
       <c r="I11" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -5502,7 +5721,7 @@
         <v>87</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
@@ -5513,7 +5732,7 @@
         <v>92</v>
       </c>
       <c r="I12" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="2:9">
@@ -5521,10 +5740,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="40"/>
@@ -5533,7 +5752,7 @@
       </c>
       <c r="H13" s="45"/>
       <c r="I13" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -5553,7 +5772,7 @@
       </c>
       <c r="H14" s="45"/>
       <c r="I14" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -5564,7 +5783,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
@@ -5573,7 +5792,7 @@
       </c>
       <c r="H15" s="45"/>
       <c r="I15" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -5581,10 +5800,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
@@ -5592,21 +5811,21 @@
         <v>12</v>
       </c>
       <c r="H16" s="43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I16" s="44" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="30">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="28.8">
       <c r="B17" s="20">
         <v>13</v>
       </c>
       <c r="C17" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>112</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
@@ -5615,18 +5834,18 @@
       </c>
       <c r="H17" s="45"/>
       <c r="I17" s="46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="28.8">
       <c r="B18" s="20">
         <v>14</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
@@ -5635,16 +5854,18 @@
       </c>
       <c r="H18" s="45"/>
       <c r="I18" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="20">
         <v>15</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="44" t="s">
-        <v>115</v>
+      <c r="C19" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="118" t="s">
+        <v>189</v>
       </c>
       <c r="E19" s="40"/>
       <c r="F19" s="40"/>
@@ -5653,16 +5874,18 @@
       </c>
       <c r="H19" s="45"/>
       <c r="I19" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="20">
         <v>16</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="44" t="s">
-        <v>96</v>
+      <c r="C20" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="118" t="s">
+        <v>190</v>
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
@@ -5671,7 +5894,7 @@
       </c>
       <c r="H20" s="45"/>
       <c r="I20" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -5689,7 +5912,7 @@
       </c>
       <c r="H21" s="45"/>
       <c r="I21" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -5700,7 +5923,7 @@
         <v>86</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
@@ -5711,7 +5934,7 @@
         <v>86</v>
       </c>
       <c r="I22" s="46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -5722,7 +5945,7 @@
         <v>85</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="40"/>
       <c r="F23" s="40"/>
@@ -5733,7 +5956,7 @@
         <v>85</v>
       </c>
       <c r="I23" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -5744,7 +5967,7 @@
         <v>87</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" s="40"/>
       <c r="F24" s="40"/>
@@ -5755,10 +5978,10 @@
         <v>87</v>
       </c>
       <c r="I24" s="44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" thickBot="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="14.7" thickBot="1">
       <c r="B25" s="24">
         <v>21</v>
       </c>
@@ -5766,7 +5989,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E25" s="40"/>
       <c r="F25" s="40"/>
@@ -5777,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="2:9">

</xml_diff>

<commit_message>
moved to a new branche and remoced the broken submodule
</commit_message>
<xml_diff>
--- a/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
+++ b/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34ABC965-A242-46AF-8020-27CD15DF7F89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="2"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23028" windowHeight="12948" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Interfaces " sheetId="1" r:id="rId1"/>
-    <sheet name="PC Command Packets" sheetId="3" r:id="rId2"/>
-    <sheet name="Functionality Checklist" sheetId="4" r:id="rId3"/>
+    <sheet name="SCROD side Signals" sheetId="1" r:id="rId1"/>
+    <sheet name="DC side signals" sheetId="6" r:id="rId2"/>
+    <sheet name="PC Command Packets" sheetId="3" r:id="rId3"/>
+    <sheet name="Functionality Checklist" sheetId="4" r:id="rId4"/>
+    <sheet name="Register" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
-  <si>
-    <t>Ethernet Module: Gigabit Transciever Interface</t>
-  </si>
-  <si>
-    <t>Register Address and Write Data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="201">
   <si>
     <t>From PC/Input Signals</t>
   </si>
@@ -33,27 +35,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>regAddr</t>
-  </si>
-  <si>
-    <t>4-bit register address</t>
-  </si>
-  <si>
-    <t>regWrData</t>
-  </si>
-  <si>
     <t xml:space="preserve">gtRx </t>
   </si>
   <si>
-    <t>16-bit register value</t>
-  </si>
-  <si>
     <t>Serial PC data in (differential)</t>
   </si>
   <si>
-    <t>Register Read Data</t>
-  </si>
-  <si>
     <t>gtClk</t>
   </si>
   <si>
@@ -69,9 +56,6 @@
     <t>To PC/Output Signals</t>
   </si>
   <si>
-    <t>regRdData</t>
-  </si>
-  <si>
     <t>current register value</t>
   </si>
   <si>
@@ -96,9 +80,6 @@
     <t>begin a register operation</t>
   </si>
   <si>
-    <t>Ethernet-Command Interpreter Interface</t>
-  </si>
-  <si>
     <t>regOp</t>
   </si>
   <si>
@@ -108,66 +89,27 @@
     <t>reset</t>
   </si>
   <si>
-    <t>Receiving Data From PC (RX)</t>
-  </si>
-  <si>
     <t>reset command from Ethernet Module</t>
   </si>
   <si>
-    <t>userRxData</t>
-  </si>
-  <si>
     <t>regAck</t>
   </si>
   <si>
     <t>Two 32-bit channels of incoming PC data</t>
   </si>
   <si>
-    <t>useRxDataValid</t>
-  </si>
-  <si>
-    <t>2-bit flag: valid incoming word</t>
-  </si>
-  <si>
-    <t xml:space="preserve">userRxDataLast </t>
-  </si>
-  <si>
-    <t>2-bit flag: last word in incoming packet</t>
-  </si>
-  <si>
-    <t>userRxdataReady</t>
-  </si>
-  <si>
     <t>Register handshake</t>
   </si>
   <si>
-    <t>2-bit flag: Interpreter ready to receive data</t>
-  </si>
-  <si>
-    <t>Sending Data to PC (TX</t>
-  </si>
-  <si>
-    <t>userTxData</t>
-  </si>
-  <si>
     <t>Two 32-bit channels of outgoing PC Data</t>
   </si>
   <si>
-    <t>useTxDataValid</t>
-  </si>
-  <si>
     <t>2-bit flag: Valid outgoing word</t>
   </si>
   <si>
-    <t xml:space="preserve">userTxDataLast </t>
-  </si>
-  <si>
     <t xml:space="preserve">2-bit flag: last word in outgoing packet </t>
   </si>
   <si>
-    <t>userTxdataReady</t>
-  </si>
-  <si>
     <t>2-bit flag: Ethernet  ready to transmit data</t>
   </si>
   <si>
@@ -198,9 +140,6 @@
     <t>0x00BE11E2</t>
   </si>
   <si>
-    <t>SCROD Register Command (single command)</t>
-  </si>
-  <si>
     <t>packet size</t>
   </si>
   <si>
@@ -210,12 +149,6 @@
     <t>0x00</t>
   </si>
   <si>
-    <t>0x00A5</t>
-  </si>
-  <si>
-    <t>Device num: SCROD RevA5 has ID "0"</t>
-  </si>
-  <si>
     <t>verbosity (31:24)</t>
   </si>
   <si>
@@ -228,15 +161,9 @@
     <t xml:space="preserve">command type </t>
   </si>
   <si>
-    <t xml:space="preserve">Ping: 0x70696e67, read: 0x72656164, write: 0x72697465 </t>
-  </si>
-  <si>
     <t>register address</t>
   </si>
   <si>
-    <t>Command data (skip for ping command)</t>
-  </si>
-  <si>
     <t>command checksum</t>
   </si>
   <si>
@@ -255,114 +182,27 @@
     <t>sum of entire words 0 to 7</t>
   </si>
   <si>
-    <t>(Read) 0x0000 or                            (Write) register value</t>
-  </si>
-  <si>
-    <t>Daughtercard Register Command</t>
-  </si>
-  <si>
     <t>Labels packet as a Register Command</t>
   </si>
   <si>
     <t>Command Interpreter-Control Register Interface</t>
   </si>
   <si>
-    <t>QB_rst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBLink reset </t>
-  </si>
-  <si>
     <t xml:space="preserve">QBLink Control Flags </t>
   </si>
   <si>
-    <t>Read output FIFO</t>
-  </si>
-  <si>
-    <t>trgLinksynced</t>
-  </si>
-  <si>
-    <t>serialClkLocked</t>
-  </si>
-  <si>
-    <t>partners clock aligned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partners synced, training state passed </t>
-  </si>
-  <si>
     <t xml:space="preserve">DC Command </t>
   </si>
   <si>
-    <t xml:space="preserve">32-bit word to be sent to DC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable write to input fifo </t>
-  </si>
-  <si>
-    <t>DC Register Data</t>
-  </si>
-  <si>
-    <t>DCResonse</t>
-  </si>
-  <si>
-    <t>32-bit response to command (non-event data)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valid Reponse </t>
-  </si>
-  <si>
-    <t>Command Interpreter-DC Communication Interface</t>
-  </si>
-  <si>
-    <t>DC Communication: QBLink Interface</t>
-  </si>
-  <si>
     <t>To DC</t>
   </si>
   <si>
-    <t>Synchronize all DC</t>
-  </si>
-  <si>
-    <t>tx_dc</t>
-  </si>
-  <si>
-    <t>sync</t>
-  </si>
-  <si>
-    <t>serial output to DC</t>
-  </si>
-  <si>
     <t>From DC</t>
   </si>
   <si>
-    <t>rx_dc</t>
-  </si>
-  <si>
-    <t>serial input from DC</t>
-  </si>
-  <si>
-    <t>QBstart_rd</t>
-  </si>
-  <si>
-    <t>QBstart_wr</t>
-  </si>
-  <si>
-    <t>dc_cmd</t>
-  </si>
-  <si>
     <t>dc_RespValid</t>
   </si>
   <si>
-    <t>DC#</t>
-  </si>
-  <si>
-    <t>0x00DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> read: 0x72656164, write: 0x72697465 </t>
-  </si>
-  <si>
     <t>Test date</t>
   </si>
   <si>
@@ -394,13 +234,471 @@
   </si>
   <si>
     <t>Read DC Reg</t>
+  </si>
+  <si>
+    <t>Register Value                                     (0x0000 for read operations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command data </t>
+  </si>
+  <si>
+    <t>packet type: device configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x70696e67</t>
+  </si>
+  <si>
+    <t>Command Type: Ping</t>
+  </si>
+  <si>
+    <t>Device label</t>
+  </si>
+  <si>
+    <t>Device #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device labels: (SCROD) 0x00A5,            (DC) 0x00DC | Device  #: 0x00 (SCROD), 0x01 through 0x08 (DC #) </t>
+  </si>
+  <si>
+    <t>Table 1. Register Command Packets</t>
+  </si>
+  <si>
+    <t>Table 2. Ping Command packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read: 0x72656164, Write: 0x72697465 </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Reg #</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>bits</t>
+  </si>
+  <si>
+    <t>11 downto 0</t>
+  </si>
+  <si>
+    <t>4 downto 0</t>
+  </si>
+  <si>
+    <t>15 downto 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 downto 0 </t>
+  </si>
+  <si>
+    <t>tx_dac_reg_data</t>
+  </si>
+  <si>
+    <t>tx_dac_load_period</t>
+  </si>
+  <si>
+    <t>tx_dac_latch_period</t>
+  </si>
+  <si>
+    <t>3 downto 0</t>
+  </si>
+  <si>
+    <t>8 downto 0</t>
+  </si>
+  <si>
+    <t>number of windows to readout</t>
+  </si>
+  <si>
+    <t>mppc dac voltage</t>
+  </si>
+  <si>
+    <t>0, 4</t>
+  </si>
+  <si>
+    <t>TargetX control reset, enables calibration</t>
+  </si>
+  <si>
+    <t>software Trigger (not implemented)</t>
+  </si>
+  <si>
+    <t>Trigger Mode (not implemented)</t>
+  </si>
+  <si>
+    <t>not used</t>
+  </si>
+  <si>
+    <t>Daughtercard FPGA Control Registers</t>
+  </si>
+  <si>
+    <t>1/2 trigger scalar count (not implemented)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2/2 trigger scalar count</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(not implemented)</t>
+    </r>
+  </si>
+  <si>
+    <t>trigger count enable(not implemented)</t>
+  </si>
+  <si>
+    <t>maximum trigger count (not implemented)</t>
+  </si>
+  <si>
+    <t>Resets stamachines</t>
+  </si>
+  <si>
+    <t>SCROD ID</t>
+  </si>
+  <si>
+    <t>dc_mask (not implemented)</t>
+  </si>
+  <si>
+    <t>output mode (not implemented)</t>
+  </si>
+  <si>
+    <t>15, 3 downto 0</t>
+  </si>
+  <si>
+    <t>enable pedestal subtraction, number of averages for calculating peds (1-7)</t>
+  </si>
+  <si>
+    <t>resets  window number during sampling, sets timing for sstin and current window count in targetX</t>
+  </si>
+  <si>
+    <t>15, 1 downto 0</t>
+  </si>
+  <si>
+    <t>15, 8 downto 0</t>
+  </si>
+  <si>
+    <t>enable use of fixed window, fixed start window</t>
+  </si>
+  <si>
+    <t>15, 8 downt 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SCROD acknowledgement wait</t>
+  </si>
+  <si>
+    <t>offset window direcion, number of windows to offset</t>
+  </si>
+  <si>
+    <t>SCROD FPGA Control Registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync Daughtercards, reset QBLink (*msb depends on how many DC you have) </t>
+  </si>
+  <si>
+    <t>8, 7* downto 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronize all DCs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signals between Command Interpreter and DC Communication </t>
+  </si>
+  <si>
+    <t>Signals between SCROD and Daughtercards</t>
+  </si>
+  <si>
+    <t>Signals between S6 Ethernet and Command Interpreter</t>
+  </si>
+  <si>
+    <t>Signals between SCROD and Gigabit Transceiver (PC Interface)</t>
+  </si>
+  <si>
+    <t>From Ethernet (RX)</t>
+  </si>
+  <si>
+    <t>To Ethernet (TX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select target DC(s) for command </t>
+  </si>
+  <si>
+    <t>Select target DC(s) for readout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DC command Type, DC register value and address</t>
+  </si>
+  <si>
+    <t>DC Status</t>
+  </si>
+  <si>
+    <t>Valid Reponse Flag</t>
+  </si>
+  <si>
+    <t>Response to register command or trigger data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evntFlag </t>
+  </si>
+  <si>
+    <t>DCResonse(32 bits)</t>
+  </si>
+  <si>
+    <t>dc_cmd (32 bits)</t>
+  </si>
+  <si>
+    <t>Sync (8 bits)</t>
+  </si>
+  <si>
+    <t>tx_dc(8 bits)</t>
+  </si>
+  <si>
+    <t>rx_dc( 8 bits)</t>
+  </si>
+  <si>
+    <t>serial input from DCs</t>
+  </si>
+  <si>
+    <t>QBLink serial output to DCs</t>
+  </si>
+  <si>
+    <t>Qbstart_wr(8 bits)</t>
+  </si>
+  <si>
+    <t>QBstart_rd(8 bits)</t>
+  </si>
+  <si>
+    <t>trgLinksynced(8 bits)</t>
+  </si>
+  <si>
+    <t>serialClkLocked(8 bits)</t>
+  </si>
+  <si>
+    <t>QB_rst(8 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select QBLink(s) to reset </t>
+  </si>
+  <si>
+    <t>QBLink partners clock aligned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBLink partners synced, training state passed </t>
+  </si>
+  <si>
+    <t>Global Event flag</t>
+  </si>
+  <si>
+    <t>regRdData(16 bits)</t>
+  </si>
+  <si>
+    <t>regAddr (16 bits)</t>
+  </si>
+  <si>
+    <t>regWrData(16 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> register value</t>
+  </si>
+  <si>
+    <t>SCROD Register Address and Write Data</t>
+  </si>
+  <si>
+    <t>SCROD Register Read Data</t>
+  </si>
+  <si>
+    <t>register address (acceptable values: 0 to 15)</t>
+  </si>
+  <si>
+    <t>useRxDataValid(2 bits)</t>
+  </si>
+  <si>
+    <t>userRxDataLast (2 bits)</t>
+  </si>
+  <si>
+    <t>userRxdataReady (2 bits)</t>
+  </si>
+  <si>
+    <t>userTxData(2 32 bit channels)</t>
+  </si>
+  <si>
+    <t>useTxDataValid (2 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userTxDataLast (2 bits) </t>
+  </si>
+  <si>
+    <t>userTxdataReady (2 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> valid incoming word flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> last word in incoming packet flag</t>
+  </si>
+  <si>
+    <t>Interpreter ready to receive data flag</t>
+  </si>
+  <si>
+    <t>userRxData (2 32 bit channels)</t>
+  </si>
+  <si>
+    <t>Packet type error: ERR_BIT_TYPE_C = x"00000002"</t>
+  </si>
+  <si>
+    <t>Packet size error: ERR_BIT_SIZE_C = x"00000001"</t>
+  </si>
+  <si>
+    <t>Invalid command target: ERR_BIT_DEST_C = x"00000004"</t>
+  </si>
+  <si>
+    <t>Invalid command type: ERR_BIT_COMM_TY_C = x"00000008"</t>
+  </si>
+  <si>
+    <t>Command checksum error: ERR_BIT_COMM_CS_C = x"00000010"</t>
+  </si>
+  <si>
+    <t>Packet checksum error: ERR_BIT_CS_C = x"00000020"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Timeout Error: ERR_BIT_TIMEOUT_C = x"00000040"</t>
+  </si>
+  <si>
+    <t>connection to DC failed: QBLINK_FAILURE_C: x"00000500"</t>
+  </si>
+  <si>
+    <t>Error Response</t>
+  </si>
+  <si>
+    <t>word#</t>
+  </si>
+  <si>
+    <t>x"00BE11E2"</t>
+  </si>
+  <si>
+    <t>x"00000005"</t>
+  </si>
+  <si>
+    <t>word_err_c = x"7768613f"</t>
+  </si>
+  <si>
+    <t>wordScrodRevC = x"0000A500"</t>
+  </si>
+  <si>
+    <t>00 &amp; commandId</t>
+  </si>
+  <si>
+    <t>errFlags</t>
+  </si>
+  <si>
+    <t>Error constants (errflags)</t>
+  </si>
+  <si>
+    <t>checksum</t>
+  </si>
+  <si>
+    <t>mppc dac address on TargetX (PCLK #)</t>
+  </si>
+  <si>
+    <t>mppc dac voltage (12-bit code)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Device labels:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (SCROD) 0x00A5, (DC) 0x00DC   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Device  #:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  (SCROD) 0x00 , (DCs) DC# or 0x0A for broadcasting to all DCs. </t>
+    </r>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Number of remaining words except packet checksum</t>
+  </si>
+  <si>
+    <t>(sending one command has 6 operations) 0x00000006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Target device is SCROD) 0x0000A500 (Broadcast to all DCs) 0x0000DC0A           </t>
+  </si>
+  <si>
+    <t>Verb(7): suppresses command response, Verb(others) = '0'. Command ID: unique ID to each command</t>
+  </si>
+  <si>
+    <t>(no verbosity) 0x00000012</t>
+  </si>
+  <si>
+    <t>(write) 0x72697465</t>
+  </si>
+  <si>
+    <t>(write value 1 to register 1) 0x00010001</t>
+  </si>
+  <si>
+    <t>0x726A7478</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -419,17 +717,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
@@ -472,8 +759,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,48 +820,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor rgb="FFC6D9F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor rgb="FFC6D9F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FFE5B8B7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor rgb="FFFBD4B4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor rgb="FFE5B8B7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -564,8 +830,56 @@
         <bgColor rgb="FFC6D9F0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE583D9"/>
+        <bgColor rgb="FFC6D9F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE583D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor rgb="FFFBD4B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor rgb="FFE5B8B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor rgb="FFE5B8B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6A8A8"/>
+        <bgColor rgb="FFC6D9F0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1042,27 +1356,27 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1074,9 +1388,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1089,9 +1401,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1101,7 +1411,100 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1110,63 +1513,9 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1175,7 +1524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1186,70 +1535,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1259,39 +1560,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1300,227 +1582,468 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF6A8A8"/>
+      <color rgb="FFE583D9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1569,7 +2092,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1602,9 +2125,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1637,6 +2177,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1812,470 +2369,490 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="32.41796875" customWidth="1"/>
+    <col min="3" max="3" width="46.15625" customWidth="1"/>
+    <col min="4" max="4" width="31.83984375" customWidth="1"/>
+    <col min="5" max="6" width="9.15625" hidden="1" customWidth="1"/>
+    <col min="7" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="89"/>
+    <row r="2" spans="2:6" ht="18.600000000000001" thickBot="1">
+      <c r="B2" s="136" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="137"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="95" t="s">
+    <row r="3" spans="2:6" ht="14.4">
+      <c r="B3" s="132" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="133"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="2:6" ht="14.4">
+      <c r="B4" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="2:6" ht="14.4">
+      <c r="B5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="9" t="s">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" ht="14.4">
+      <c r="B6" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" ht="14.7" thickBot="1">
+      <c r="B7" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" ht="14.4">
+      <c r="B8" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="139"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:6" ht="14.4">
+      <c r="B9" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="14.4">
+      <c r="B10" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="2:6" ht="30.75" thickBot="1">
-      <c r="B7" s="13" t="s">
+    </row>
+    <row r="11" spans="2:6" ht="14.7" thickBot="1">
+      <c r="B11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="99" t="s">
+      <c r="C11" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B11" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="19.5" thickBot="1">
-      <c r="B14" s="98" t="s">
+    </row>
+    <row r="14" spans="2:6" ht="18.600000000000001" thickBot="1">
+      <c r="B14" s="136" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="137"/>
+    </row>
+    <row r="15" spans="2:6" ht="14.4">
+      <c r="B15" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="133"/>
+    </row>
+    <row r="16" spans="2:6" ht="14.4">
+      <c r="B16" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="14.4">
+      <c r="B17" s="98" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="14.4">
+      <c r="B18" s="98" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="102" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="14.4">
+      <c r="B19" s="98" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" s="102" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="14.7" thickBot="1">
+      <c r="B20" s="99" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="103" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B21" s="134" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="135"/>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B22" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B23" s="100" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B24" s="100" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="89"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="96"/>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="30">
-      <c r="B17" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="30">
-      <c r="B19" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="30">
-      <c r="B20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="97" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="91"/>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B22" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B23" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B24" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B25" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B26" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>50</v>
+      <c r="B25" s="100" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B26" s="101" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="28" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="29" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B29" s="88" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="89"/>
+      <c r="B29" s="140" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="141"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B30" s="90" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="91"/>
+      <c r="B30" s="142" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="143"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" customHeight="1">
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
+      <c r="B32" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="95" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>9</v>
+      <c r="B33" s="96" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="97" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="92" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="91"/>
+      <c r="B34" s="144" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="145"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B35" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>4</v>
+      <c r="B35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B37" s="146" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="145"/>
+    </row>
+    <row r="38" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="20" t="s">
+    </row>
+    <row r="39" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B39" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B37" s="93" t="s">
+      <c r="C39" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="30" customHeight="1">
+      <c r="B40" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="91"/>
-    </row>
-    <row r="38" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B38" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B39" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="30" customHeight="1">
-      <c r="B40" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>31</v>
+      <c r="C40" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B41" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>40</v>
+      <c r="B41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="43" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B44" s="94" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" s="89"/>
+      <c r="B44" s="147" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="148"/>
     </row>
     <row r="45" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B45" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="79"/>
+      <c r="B45" s="151" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="152"/>
     </row>
     <row r="46" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B46" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="53" t="s">
-        <v>4</v>
+      <c r="B46" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="75" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B47" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="55" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B48" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" s="40" customFormat="1" ht="30" customHeight="1">
-      <c r="B49" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="57" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B50" s="75" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" s="58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B51" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" s="81"/>
+      <c r="B47" s="90" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="91" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B48" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="92" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" s="15" customFormat="1" ht="30" customHeight="1">
+      <c r="B49" s="89" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="92" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B50" s="89" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B51" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="78" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="52" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B52" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B53" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" s="62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B54" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="62" t="s">
-        <v>93</v>
+      <c r="B52" s="153" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="154"/>
+    </row>
+    <row r="53" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B53" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B54" s="81" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="82" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B55" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="83"/>
-    </row>
-    <row r="56" spans="2:3" ht="30" customHeight="1">
-      <c r="B56" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="64" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B57" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="65" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="59" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="60" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B60" s="84" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="85"/>
-    </row>
-    <row r="61" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B61" s="86" t="s">
-        <v>100</v>
-      </c>
-      <c r="C61" s="87"/>
-    </row>
-    <row r="62" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B62" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="68" t="s">
-        <v>4</v>
-      </c>
+      <c r="B55" s="155" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="156"/>
+    </row>
+    <row r="56" spans="2:3" ht="15" customHeight="1">
+      <c r="B56" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B57" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="109" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B58" s="108" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="109" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B59" s="110" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="111" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" ht="12" customHeight="1">
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+    </row>
+    <row r="61" spans="2:3" ht="21" customHeight="1">
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+    </row>
+    <row r="62" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B62" s="157" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="158"/>
     </row>
     <row r="63" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B63" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" s="70" t="s">
-        <v>101</v>
-      </c>
+      <c r="B63" s="159" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="160"/>
     </row>
     <row r="64" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B64" s="69" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="70" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B65" s="76" t="s">
-        <v>105</v>
-      </c>
-      <c r="C65" s="77"/>
-    </row>
-    <row r="66" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B66" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B67" s="73" t="s">
-        <v>106</v>
-      </c>
-      <c r="C67" s="74" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="69" spans="2:3" ht="15.75" customHeight="1"/>
+      <c r="B64" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B65" s="85" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="86" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B66" s="104" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="105" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B67" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" s="150"/>
+    </row>
+    <row r="68" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B68" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B69" s="87" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" s="88" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="70" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="71" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="72" spans="2:3" ht="15.75" customHeight="1"/>
@@ -3211,23 +3788,23 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3235,382 +3812,508 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:T999"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="16.41796875" customWidth="1"/>
+    <col min="3" max="3" width="16.15625" customWidth="1"/>
+    <col min="4" max="4" width="13.15625" customWidth="1"/>
+    <col min="5" max="5" width="16.26171875" customWidth="1"/>
+    <col min="6" max="6" width="37.15625" style="115" customWidth="1"/>
+    <col min="7" max="7" width="37.41796875" customWidth="1"/>
+    <col min="8" max="14" width="8.68359375" customWidth="1"/>
+    <col min="15" max="15" width="35.15625" customWidth="1"/>
+    <col min="16" max="16" width="58.41796875" customWidth="1"/>
+    <col min="17" max="27" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="105" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="110" t="s">
+    <row r="2" spans="1:20" ht="15" customHeight="1" thickBot="1">
+      <c r="B2" s="167" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="114"/>
+      <c r="N2" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="P2" s="112" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1">
+      <c r="A3" s="168" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="176" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="176"/>
+      <c r="F3" s="177" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="173" t="s">
+        <v>192</v>
+      </c>
+      <c r="N3" s="52">
+        <v>0</v>
+      </c>
+      <c r="O3" s="113" t="s">
+        <v>181</v>
+      </c>
+      <c r="P3" s="113" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1">
+      <c r="A4" s="169"/>
+      <c r="B4" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="178"/>
+      <c r="G4" s="174"/>
+      <c r="N4" s="52">
+        <v>1</v>
+      </c>
+      <c r="O4" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="P4" s="113" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1">
+      <c r="A5" s="20">
+        <v>0</v>
+      </c>
+      <c r="B5" s="170" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="128" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="52">
+        <v>2</v>
+      </c>
+      <c r="O5" s="113" t="s">
+        <v>183</v>
+      </c>
+      <c r="P5" s="113" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="30" customHeight="1">
+      <c r="A6" s="20">
+        <v>1</v>
+      </c>
+      <c r="B6" s="170" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="171"/>
+      <c r="D6" s="171"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="123" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" s="116" t="s">
+        <v>194</v>
+      </c>
+      <c r="N6" s="52">
+        <v>3</v>
+      </c>
+      <c r="O6" s="113" t="s">
+        <v>184</v>
+      </c>
+      <c r="P6" s="113" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15" customHeight="1">
+      <c r="A7" s="20">
+        <v>2</v>
+      </c>
+      <c r="B7" s="170" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="171"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="123" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="129" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="52"/>
+      <c r="O7" s="113" t="s">
+        <v>185</v>
+      </c>
+      <c r="P7" s="113" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="26" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A8" s="20">
+        <v>3</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="170" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="172"/>
+      <c r="E8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="121" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="131" t="s">
+        <v>195</v>
+      </c>
+      <c r="N8" s="52">
+        <v>5</v>
+      </c>
+      <c r="O8" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="P8" s="113" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="45" customHeight="1">
+      <c r="A9" s="20">
+        <v>4</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="161" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="162"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="123" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="130" t="s">
+        <v>197</v>
+      </c>
+      <c r="N9" s="52">
+        <v>6</v>
+      </c>
+      <c r="O9" s="113" t="s">
+        <v>188</v>
+      </c>
+      <c r="P9" s="113" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="30" customHeight="1">
+      <c r="A10" s="20">
+        <v>5</v>
+      </c>
+      <c r="B10" s="161" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="162"/>
+      <c r="D10" s="162"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="121" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="130" t="s">
+        <v>198</v>
+      </c>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="113" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="30" customHeight="1">
+      <c r="A11" s="20">
+        <v>6</v>
+      </c>
+      <c r="B11" s="161" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="163"/>
+      <c r="D11" s="175" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="163"/>
+      <c r="F11" s="121" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="130" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15" customHeight="1">
+      <c r="A12" s="20">
+        <v>7</v>
+      </c>
+      <c r="B12" s="161" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="162"/>
+      <c r="D12" s="162"/>
+      <c r="E12" s="163"/>
+      <c r="F12" s="121" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="130" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15" customHeight="1" thickBot="1">
+      <c r="A13" s="24">
+        <v>8</v>
+      </c>
+      <c r="B13" s="164" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="165"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="109" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="109"/>
-      <c r="F3" s="100" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="111"/>
-      <c r="B4" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="101"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="45">
+      <c r="G13" s="130"/>
+    </row>
+    <row r="14" spans="1:20" ht="15" customHeight="1">
+      <c r="T14" s="42" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" thickBot="1">
+      <c r="A16" s="26"/>
+      <c r="B16" s="167" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="167"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1">
+      <c r="A17" s="168" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="176" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="176"/>
+      <c r="D17" s="176" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="176"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="179" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1">
+      <c r="A18" s="169"/>
+      <c r="B18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="127"/>
+      <c r="G18" s="180"/>
+    </row>
+    <row r="19" spans="1:14" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="20">
         <v>0</v>
       </c>
-      <c r="B5" s="102" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="46" t="s">
+      <c r="B19" s="170" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="170" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="171"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A21" s="20">
+        <v>2</v>
+      </c>
+      <c r="B21" s="170" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="171"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="172"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="45" customHeight="1">
+      <c r="A22" s="20">
+        <v>3</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="170" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="172"/>
+      <c r="E22" s="17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="A6" s="45">
-        <v>1</v>
-      </c>
-      <c r="B6" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="47" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="45">
-        <v>2</v>
-      </c>
-      <c r="B7" s="102" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="47" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
-      <c r="A8" s="45">
-        <v>3</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="102" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="104"/>
-      <c r="E8" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" customHeight="1">
-      <c r="A9" s="45">
+      <c r="F22" s="123"/>
+      <c r="G22" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" customHeight="1">
+      <c r="A23" s="20">
         <v>4</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="112"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
-      <c r="A10" s="45">
+      <c r="B23" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="161" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="162"/>
+      <c r="E23" s="163"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" customHeight="1">
+      <c r="A24" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="106" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
-      <c r="A11" s="45">
+      <c r="B24" s="161" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="162"/>
+      <c r="D24" s="162"/>
+      <c r="E24" s="163"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="N24" s="42"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A25" s="20">
         <v>6</v>
       </c>
-      <c r="B11" s="106" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="107"/>
-      <c r="D11" s="108" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="107"/>
-      <c r="F11" s="48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="45">
+      <c r="B25" s="161" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="162"/>
+      <c r="D25" s="162"/>
+      <c r="E25" s="163"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A26" s="24">
         <v>7</v>
       </c>
-      <c r="B12" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="48" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="49">
-        <v>8</v>
-      </c>
-      <c r="B13" s="113" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B15" s="116" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
-      <c r="A16" s="110" t="s">
+      <c r="B26" s="164" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="165"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="126"/>
+      <c r="G26" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="109" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="109"/>
-      <c r="F16" s="100" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
-      <c r="A17" s="111"/>
-      <c r="B17" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="101"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="45">
-        <v>0</v>
-      </c>
-      <c r="B18" s="102" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="103"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="44" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="51">
-        <v>1</v>
-      </c>
-      <c r="B19" s="106" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="48" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="51">
-        <v>2</v>
-      </c>
-      <c r="B20" s="106" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="48" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="45">
-        <v>3</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="102" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" s="104"/>
-      <c r="E21" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1">
-      <c r="A22" s="45">
-        <v>4</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="112"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1">
-      <c r="A23" s="45">
-        <v>5</v>
-      </c>
-      <c r="B23" s="106" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="112"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="48" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="45">
-        <v>6</v>
-      </c>
-      <c r="B24" s="106" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="107"/>
-      <c r="D24" s="108" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="107"/>
-      <c r="F24" s="48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A25" s="45">
-        <v>7</v>
-      </c>
-      <c r="B25" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="48" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="49">
-        <v>8</v>
-      </c>
-      <c r="B26" s="113" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="114"/>
-      <c r="D26" s="114"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="33" ht="30" customHeight="1"/>
+    <row r="34" ht="30" customHeight="1"/>
+    <row r="35" ht="47.25" customHeight="1"/>
+    <row r="36" ht="30.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -4574,32 +5277,21 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
+  <mergeCells count="29">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B19:E19"/>
     <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B11:C11"/>
@@ -4607,173 +5299,744 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.68359375" customWidth="1"/>
+    <col min="3" max="3" width="20.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:3" ht="14.7" thickBot="1"/>
     <row r="3" spans="2:3">
-      <c r="B3" s="117" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="118" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="30.75" thickBot="1">
-      <c r="B4" s="128" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="129">
+      <c r="B3" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="29.1" thickBot="1">
+      <c r="B4" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="39">
         <v>43579</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B5" s="126" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="127" t="s">
-        <v>119</v>
+    <row r="5" spans="2:3" ht="14.7" thickBot="1">
+      <c r="B5" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="124" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="125"/>
+      <c r="B6" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="119" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="121"/>
+      <c r="B7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="119" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="121"/>
+      <c r="B8" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="119" t="s">
-        <v>123</v>
-      </c>
-      <c r="C9" s="121"/>
+      <c r="B9" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="119" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="121"/>
+      <c r="B10" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="119" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="121"/>
+      <c r="B11" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="120"/>
-      <c r="C12" s="121"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="120"/>
-      <c r="C13" s="121"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="120"/>
-      <c r="C14" s="121"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="120"/>
-      <c r="C15" s="121"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="120"/>
-      <c r="C16" s="121"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="120"/>
-      <c r="C17" s="121"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="120"/>
-      <c r="C18" s="121"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="120"/>
-      <c r="C19" s="121"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="120"/>
-      <c r="C20" s="121"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
     </row>
     <row r="21" spans="2:3">
-      <c r="B21" s="120"/>
-      <c r="C21" s="121"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="2:3">
-      <c r="B22" s="120"/>
-      <c r="C22" s="121"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
     </row>
     <row r="23" spans="2:3">
-      <c r="B23" s="120"/>
-      <c r="C23" s="121"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="2:3">
-      <c r="B24" s="120"/>
-      <c r="C24" s="121"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="120"/>
-      <c r="C25" s="121"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="120"/>
-      <c r="C26" s="121"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="120"/>
-      <c r="C27" s="121"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="120"/>
-      <c r="C28" s="121"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="29" spans="2:3">
-      <c r="B29" s="120"/>
-      <c r="C29" s="121"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="120"/>
-      <c r="C30" s="121"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="120"/>
-      <c r="C31" s="121"/>
-    </row>
-    <row r="32" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B32" s="122"/>
-      <c r="C32" s="123"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+    </row>
+    <row r="32" spans="2:3" ht="14.7" thickBot="1">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B2:I28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="18.15625" customWidth="1"/>
+    <col min="4" max="4" width="55" customWidth="1"/>
+    <col min="7" max="7" width="9.41796875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="51.26171875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1">
+      <c r="B2" s="147" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="G2" s="181" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="20">
+        <v>0</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="54">
+        <v>0</v>
+      </c>
+      <c r="H4" s="55">
+        <v>0</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="20">
+        <v>1</v>
+      </c>
+      <c r="H5" s="45">
+        <v>0</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="28.8">
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="20">
+        <v>2</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="20">
+        <v>3</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="20">
+        <v>3</v>
+      </c>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="20">
+        <v>4</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="20">
+        <v>4</v>
+      </c>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="20">
+        <v>5</v>
+      </c>
+      <c r="C9" s="45">
+        <v>0</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="20">
+        <v>5</v>
+      </c>
+      <c r="H9" s="45">
+        <v>0</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="20">
+        <v>6</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="20">
+        <v>6</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="20">
+        <v>7</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="20">
+        <v>7</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="20">
+        <v>8</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="20">
+        <v>8</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="20">
+        <v>9</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="20">
+        <v>9</v>
+      </c>
+      <c r="H13" s="45"/>
+      <c r="I13" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="20">
+        <v>10</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="20">
+        <v>10</v>
+      </c>
+      <c r="H14" s="45"/>
+      <c r="I14" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="20">
+        <v>11</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="20">
+        <v>11</v>
+      </c>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="20">
+        <v>12</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="20">
+        <v>12</v>
+      </c>
+      <c r="H16" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="I16" s="44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="28.8">
+      <c r="B17" s="20">
+        <v>13</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="20">
+        <v>13</v>
+      </c>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="28.8">
+      <c r="B18" s="20">
+        <v>14</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="20">
+        <v>14</v>
+      </c>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="20">
+        <v>15</v>
+      </c>
+      <c r="C19" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="20">
+        <v>15</v>
+      </c>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="20">
+        <v>16</v>
+      </c>
+      <c r="C20" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="118" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="20">
+        <v>16</v>
+      </c>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="20">
+        <v>17</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="20">
+        <v>17</v>
+      </c>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="20">
+        <v>18</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="20">
+        <v>18</v>
+      </c>
+      <c r="H22" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="20">
+        <v>19</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="20">
+        <v>19</v>
+      </c>
+      <c r="H23" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" s="46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="20">
+        <v>20</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="20">
+        <v>20</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="14.7" thickBot="1">
+      <c r="B25" s="24">
+        <v>21</v>
+      </c>
+      <c r="C25" s="47">
+        <v>0</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="24">
+        <v>21</v>
+      </c>
+      <c r="H25" s="47">
+        <v>0</v>
+      </c>
+      <c r="I25" s="48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="53"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+    </row>
+  </sheetData>
+  <sortState ref="B4:G27">
+    <sortCondition ref="B4:B27"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First commit, add FW Guide and updated FPGA signal tables
</commit_message>
<xml_diff>
--- a/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
+++ b/EIC-Beamtest-FW/Documentation/HMB_SCROD_FPGAsignals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34ABC965-A242-46AF-8020-27CD15DF7F89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1B1E4F-01F5-435F-A802-C8F8925228A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23028" windowHeight="12948" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCROD side Signals" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,12 @@
     <sheet name="Register" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="201">
-  <si>
-    <t>From PC/Input Signals</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="249">
   <si>
     <t>Signal</t>
   </si>
@@ -53,9 +51,6 @@
     <t>Alternative Clock, used in fabric (differential)</t>
   </si>
   <si>
-    <t>To PC/Output Signals</t>
-  </si>
-  <si>
     <t>current register value</t>
   </si>
   <si>
@@ -183,9 +178,6 @@
   </si>
   <si>
     <t>Labels packet as a Register Command</t>
-  </si>
-  <si>
-    <t>Command Interpreter-Control Register Interface</t>
   </si>
   <si>
     <t xml:space="preserve">QBLink Control Flags </t>
@@ -411,9 +403,6 @@
     <t>offset window direcion, number of windows to offset</t>
   </si>
   <si>
-    <t>SCROD FPGA Control Registers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sync Daughtercards, reset QBLink (*msb depends on how many DC you have) </t>
   </si>
   <si>
@@ -423,18 +412,6 @@
     <t xml:space="preserve">Synchronize all DCs </t>
   </si>
   <si>
-    <t xml:space="preserve">Signals between Command Interpreter and DC Communication </t>
-  </si>
-  <si>
-    <t>Signals between SCROD and Daughtercards</t>
-  </si>
-  <si>
-    <t>Signals between S6 Ethernet and Command Interpreter</t>
-  </si>
-  <si>
-    <t>Signals between SCROD and Gigabit Transceiver (PC Interface)</t>
-  </si>
-  <si>
     <t>From Ethernet (RX)</t>
   </si>
   <si>
@@ -591,21 +568,12 @@
     <t>connection to DC failed: QBLINK_FAILURE_C: x"00000500"</t>
   </si>
   <si>
-    <t>Error Response</t>
-  </si>
-  <si>
-    <t>word#</t>
-  </si>
-  <si>
     <t>x"00BE11E2"</t>
   </si>
   <si>
     <t>x"00000005"</t>
   </si>
   <si>
-    <t>word_err_c = x"7768613f"</t>
-  </si>
-  <si>
     <t>wordScrodRevC = x"0000A500"</t>
   </si>
   <si>
@@ -615,16 +583,7 @@
     <t>errFlags</t>
   </si>
   <si>
-    <t>Error constants (errflags)</t>
-  </si>
-  <si>
     <t>checksum</t>
-  </si>
-  <si>
-    <t>mppc dac address on TargetX (PCLK #)</t>
-  </si>
-  <si>
-    <t>mppc dac voltage (12-bit code)</t>
   </si>
   <si>
     <r>
@@ -693,12 +652,198 @@
   <si>
     <t>0x726A7478</t>
   </si>
+  <si>
+    <t>Table 1. Signals between SCROD and Gigabit Transceiver (PC Interface)</t>
+  </si>
+  <si>
+    <t>Table 2. Signals between S6 Ethernet and Command Interpreter</t>
+  </si>
+  <si>
+    <t>Table 3. Command Interpreter-Control Register Interface</t>
+  </si>
+  <si>
+    <t>PC DATA IN</t>
+  </si>
+  <si>
+    <t>PC DATA OUT</t>
+  </si>
+  <si>
+    <t>Table 4. SCROD FPGA Control Registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 5. Signals between Command Interpreter and DC Communication </t>
+  </si>
+  <si>
+    <t>Table 6. Signals between SCROD and Daughtercards</t>
+  </si>
+  <si>
+    <t>Error Response Packet</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Error Constants (errFlags)</t>
+  </si>
+  <si>
+    <t>Register Write Response</t>
+  </si>
+  <si>
+    <t>x"00000006"</t>
+  </si>
+  <si>
+    <t>WORD_ERR_C = x"7768613f"</t>
+  </si>
+  <si>
+    <t>WORD_ERR_C = 0x7768613f.</t>
+  </si>
+  <si>
+    <t>00 &amp; commandID</t>
+  </si>
+  <si>
+    <t>WORD_WRITE_C =</t>
+  </si>
+  <si>
+    <t>r.regWrData &amp; r.regAddr</t>
+  </si>
+  <si>
+    <t>WORD_READ_C = x"72656164"</t>
+  </si>
+  <si>
+    <t>Register Read Response</t>
+  </si>
+  <si>
+    <t>Error Flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trim DAC voltage </t>
+  </si>
+  <si>
+    <t>Trim DAC address</t>
+  </si>
+  <si>
+    <t>Table 13. Signals Included in RegType record</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Statemachine states</t>
+  </si>
+  <si>
+    <t>regAddr</t>
+  </si>
+  <si>
+    <t>regWrData</t>
+  </si>
+  <si>
+    <t>regRdData</t>
+  </si>
+  <si>
+    <t>sendResp</t>
+  </si>
+  <si>
+    <t>rxDataReady</t>
+  </si>
+  <si>
+    <t>txData</t>
+  </si>
+  <si>
+    <t>txDataValid</t>
+  </si>
+  <si>
+    <t>txDataLast</t>
+  </si>
+  <si>
+    <t>wordsLeft</t>
+  </si>
+  <si>
+    <t>wordOutCnt</t>
+  </si>
+  <si>
+    <t>deviceID</t>
+  </si>
+  <si>
+    <t>commandType</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>commandID</t>
+  </si>
+  <si>
+    <t>noResponse</t>
+  </si>
+  <si>
+    <t>timeoutCnt</t>
+  </si>
+  <si>
+    <t>logic vector(31 downto 0)</t>
+  </si>
+  <si>
+    <t>standard logic bit</t>
+  </si>
+  <si>
+    <t>Register data to writelogic vector(REG_BIT_DATA_G-1 downto 0)</t>
+  </si>
+  <si>
+    <t>words left in packet, logic vector(31 downto 0)</t>
+  </si>
+  <si>
+    <t># of words sent to PC, logic vector(7 downto 0)</t>
+  </si>
+  <si>
+    <t>setting to disable SCROD response to PC, standard logic bit</t>
+  </si>
+  <si>
+    <t>Timer for timeout error, logic vector(31 downto 0)</t>
+  </si>
+  <si>
+    <t>REG_ADDR_BITS_G</t>
+  </si>
+  <si>
+    <t>TIMEOUT_G</t>
+  </si>
+  <si>
+    <t>GATE_DELAY_G</t>
+  </si>
+  <si>
+    <t>num_DC</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>FPGA register address, logic vector(REG_ADDR_BITS_G-1 downto 0)</t>
+  </si>
+  <si>
+    <t>Read register value, logic vector(REG_BIT_DATA_G-1 downto 0)</t>
+  </si>
+  <si>
+    <t>REG_DATA_BITS_G</t>
+  </si>
+  <si>
+    <t>length of register data, integer</t>
+  </si>
+  <si>
+    <t>length of register address, integer</t>
+  </si>
+  <si>
+    <t>number of clock cycles to wait for register response, integer</t>
+  </si>
+  <si>
+    <t>time (ns)</t>
+  </si>
+  <si>
+    <t>number of DCs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -779,6 +924,26 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="17">
@@ -879,7 +1044,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1520,11 +1685,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1825,12 +2046,6 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1881,6 +2096,53 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1962,6 +2224,15 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2014,6 +2285,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2025,6 +2299,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2370,16 +2671,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F1002"/>
+  <dimension ref="A2:F1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.68359375" customWidth="1"/>
-    <col min="2" max="2" width="32.41796875" customWidth="1"/>
+    <col min="1" max="1" width="19.7890625" customWidth="1"/>
+    <col min="2" max="2" width="33.83984375" customWidth="1"/>
     <col min="3" max="3" width="46.15625" customWidth="1"/>
     <col min="4" max="4" width="31.83984375" customWidth="1"/>
     <col min="5" max="6" width="9.15625" hidden="1" customWidth="1"/>
@@ -2387,404 +2688,404 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="18.600000000000001" thickBot="1">
-      <c r="B2" s="136" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="137"/>
+      <c r="B2" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="152"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="14.4">
-      <c r="B3" s="132" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="133"/>
+      <c r="B3" s="147" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="148"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="2:6" ht="14.4">
       <c r="B4" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>2</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="2:6" ht="14.4">
       <c r="B5" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="67" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>4</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:6" ht="14.4">
       <c r="B6" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="59" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" s="59" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:6" ht="14.7" thickBot="1">
       <c r="B7" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="69" t="s">
-        <v>8</v>
-      </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="2:6" ht="14.4">
-      <c r="B8" s="138" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="139"/>
+      <c r="B8" s="153" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="154"/>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="2:6" ht="14.4">
       <c r="B9" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="71" t="s">
         <v>1</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="14.4">
       <c r="B10" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="72" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="14.7" thickBot="1">
       <c r="B11" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="73" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="14" spans="2:6" ht="18.600000000000001" thickBot="1">
-      <c r="B14" s="136" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="137"/>
+      <c r="B14" s="151" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="152"/>
     </row>
     <row r="15" spans="2:6" ht="14.4">
-      <c r="B15" s="132" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="133"/>
+      <c r="B15" s="147" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="148"/>
     </row>
     <row r="16" spans="2:6" ht="14.4">
       <c r="B16" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="66" t="s">
         <v>1</v>
-      </c>
-      <c r="C16" s="66" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="14.4">
       <c r="B17" s="98" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C17" s="59" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="14.4">
       <c r="B18" s="98" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C18" s="102" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="14.4">
       <c r="B19" s="98" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C19" s="102" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="14.7" thickBot="1">
       <c r="B20" s="99" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C20" s="103" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="134" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" s="135"/>
+      <c r="B21" s="149" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="150"/>
     </row>
     <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="71" t="s">
         <v>1</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15.75" customHeight="1">
       <c r="B23" s="100" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="15.75" customHeight="1">
       <c r="B24" s="100" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" customHeight="1">
       <c r="B25" s="100" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B26" s="101" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C26" s="64" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="28" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="29" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B29" s="140" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="141"/>
+      <c r="B29" s="155" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="156"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B30" s="142" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="143"/>
+      <c r="B30" s="157" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="158"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" customHeight="1">
       <c r="B31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15.75" customHeight="1">
       <c r="B32" s="94" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C32" s="95" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B33" s="96" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C33" s="97" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="144" t="s">
-        <v>157</v>
-      </c>
-      <c r="C34" s="145"/>
+      <c r="B34" s="159" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="160"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>1</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B36" s="93" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C36" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B37" s="161" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B37" s="146" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="145"/>
+      <c r="C37" s="160"/>
     </row>
     <row r="38" spans="2:3" ht="15.75" customHeight="1">
       <c r="B38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.75" customHeight="1">
       <c r="B39" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="30" customHeight="1">
       <c r="B40" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B41" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>22</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="43" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B44" s="147" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" s="148"/>
+      <c r="B44" s="162" t="s">
+        <v>193</v>
+      </c>
+      <c r="C44" s="163"/>
     </row>
     <row r="45" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B45" s="151" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="152"/>
+      <c r="B45" s="166" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="167"/>
     </row>
     <row r="46" spans="2:3" ht="15.75" customHeight="1">
       <c r="B46" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="75" t="s">
         <v>1</v>
-      </c>
-      <c r="C46" s="75" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15.75" customHeight="1">
       <c r="B47" s="90" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C47" s="91" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="B48" s="89" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C48" s="92" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="2:3" s="15" customFormat="1" ht="30" customHeight="1">
       <c r="B49" s="89" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C49" s="92" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="15.75" customHeight="1">
       <c r="B50" s="89" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C50" s="76" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B51" s="77" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C51" s="78" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B52" s="153" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="154"/>
+      <c r="B52" s="168" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="169"/>
     </row>
     <row r="53" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="B53" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="80" t="s">
         <v>1</v>
-      </c>
-      <c r="C53" s="80" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="54" spans="2:3" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="B54" s="81" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C54" s="82" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B55" s="155" t="s">
-        <v>132</v>
-      </c>
-      <c r="C55" s="156"/>
+      <c r="B55" s="170" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="171"/>
     </row>
     <row r="56" spans="2:3" ht="15" customHeight="1">
       <c r="B56" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="107" t="s">
         <v>1</v>
-      </c>
-      <c r="C56" s="107" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15.75" customHeight="1">
       <c r="B57" s="108" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C57" s="109" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="15.75" customHeight="1">
       <c r="B58" s="108" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C58" s="109" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B59" s="110" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C59" s="111" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="12" customHeight="1">
@@ -2796,106 +3097,307 @@
       <c r="C61" s="57"/>
     </row>
     <row r="62" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B62" s="157" t="s">
-        <v>124</v>
-      </c>
-      <c r="C62" s="158"/>
+      <c r="B62" s="172" t="s">
+        <v>194</v>
+      </c>
+      <c r="C62" s="173"/>
     </row>
     <row r="63" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B63" s="159" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="160"/>
+      <c r="B63" s="174" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" s="175"/>
     </row>
     <row r="64" spans="2:3" ht="15.75" customHeight="1">
       <c r="B64" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="84" t="s">
         <v>1</v>
-      </c>
-      <c r="C64" s="84" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15.75" customHeight="1">
       <c r="B65" s="85" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C65" s="86" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B66" s="104" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C66" s="105" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B67" s="149" t="s">
-        <v>57</v>
-      </c>
-      <c r="C67" s="150"/>
+      <c r="B67" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="165"/>
     </row>
     <row r="68" spans="2:3" ht="15.75" customHeight="1">
       <c r="B68" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="107" t="s">
         <v>1</v>
-      </c>
-      <c r="C68" s="107" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="B69" s="87" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C69" s="88" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="71" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="72" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="73" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="74" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="75" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="76" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="77" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="78" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="79" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="80" spans="2:3" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="72" spans="2:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B72" s="151" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" s="151"/>
+    </row>
+    <row r="73" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B73" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B74" s="203" t="s">
+        <v>211</v>
+      </c>
+      <c r="C74" s="23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="24.3" customHeight="1">
+      <c r="B75" s="203" t="s">
+        <v>213</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="29.4" customHeight="1">
+      <c r="B76" s="204" t="s">
+        <v>214</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="28.2" customHeight="1">
+      <c r="B77" s="204" t="s">
+        <v>215</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B78" s="204" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B79" s="204" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B80" s="204" t="s">
+        <v>216</v>
+      </c>
+      <c r="C80" s="205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B81" s="204" t="s">
+        <v>217</v>
+      </c>
+      <c r="C81" s="205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B82" s="204" t="s">
+        <v>218</v>
+      </c>
+      <c r="C82" s="205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B83" s="204" t="s">
+        <v>219</v>
+      </c>
+      <c r="C83" s="205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B84" s="204" t="s">
+        <v>220</v>
+      </c>
+      <c r="C84" s="205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B85" s="204" t="s">
+        <v>221</v>
+      </c>
+      <c r="C85" s="23" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B86" s="204" t="s">
+        <v>222</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B87" s="204" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="205" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B88" s="204" t="s">
+        <v>223</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B89" s="204" t="s">
+        <v>224</v>
+      </c>
+      <c r="C89" s="205" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B90" s="204" t="s">
+        <v>225</v>
+      </c>
+      <c r="C90" s="205" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B91" s="204" t="s">
+        <v>226</v>
+      </c>
+      <c r="C91" s="205" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B92" s="204" t="s">
+        <v>227</v>
+      </c>
+      <c r="C92" s="23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B93" s="204" t="s">
+        <v>175</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B94" s="206" t="s">
+        <v>228</v>
+      </c>
+      <c r="C94" s="207" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="96" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A96" s="146" t="s">
+        <v>240</v>
+      </c>
+      <c r="B96" s="208" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A97" t="s">
+        <v>236</v>
+      </c>
+      <c r="B97" s="209" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A98" t="s">
+        <v>243</v>
+      </c>
+      <c r="B98" s="209" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="32.1" customHeight="1">
+      <c r="A99" s="131" t="s">
+        <v>237</v>
+      </c>
+      <c r="B99" s="210" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A100" s="131" t="s">
+        <v>238</v>
+      </c>
+      <c r="B100" s="202" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A101" s="131" t="s">
+        <v>239</v>
+      </c>
+      <c r="B101" s="202" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="103" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="104" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="105" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="106" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="107" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="108" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="109" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="110" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="111" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="112" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="113" ht="15.75" customHeight="1"/>
     <row r="114" ht="15.75" customHeight="1"/>
     <row r="115" ht="15.75" customHeight="1"/>
@@ -3787,7 +4289,8 @@
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="B72:C72"/>
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B52:C52"/>
@@ -3816,7 +4319,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3827,173 +4330,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:T999"/>
+  <dimension ref="A1:T999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView topLeftCell="F1" zoomScale="58" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.68359375" customWidth="1"/>
-    <col min="2" max="2" width="16.41796875" customWidth="1"/>
-    <col min="3" max="3" width="16.15625" customWidth="1"/>
-    <col min="4" max="4" width="13.15625" customWidth="1"/>
-    <col min="5" max="5" width="16.26171875" customWidth="1"/>
-    <col min="6" max="6" width="37.15625" style="115" customWidth="1"/>
-    <col min="7" max="7" width="37.41796875" customWidth="1"/>
+    <col min="2" max="2" width="14.89453125" customWidth="1"/>
+    <col min="3" max="3" width="13.41796875" customWidth="1"/>
+    <col min="4" max="4" width="11.68359375" customWidth="1"/>
+    <col min="5" max="5" width="12.89453125" customWidth="1"/>
+    <col min="6" max="6" width="21.3671875" style="113" customWidth="1"/>
+    <col min="7" max="7" width="21.89453125" customWidth="1"/>
     <col min="8" max="14" width="8.68359375" customWidth="1"/>
     <col min="15" max="15" width="35.15625" customWidth="1"/>
     <col min="16" max="16" width="58.41796875" customWidth="1"/>
     <col min="17" max="27" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:20" ht="15" customHeight="1" thickBot="1">
+      <c r="N1" s="176" t="s">
+        <v>195</v>
+      </c>
+      <c r="O1" s="176"/>
+      <c r="P1" s="146" t="s">
+        <v>207</v>
+      </c>
+    </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="167" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="114"/>
-      <c r="N2" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="O2" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="P2" s="112" t="s">
-        <v>187</v>
+      <c r="B2" s="185" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="112"/>
+      <c r="N2" s="137" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="138" t="s">
+        <v>196</v>
+      </c>
+      <c r="P2" s="134" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="186" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="194" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="176" t="s">
+      <c r="E3" s="194"/>
+      <c r="F3" s="195" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176" t="s">
+      <c r="G3" s="191" t="s">
+        <v>178</v>
+      </c>
+      <c r="N3" s="139">
+        <v>0</v>
+      </c>
+      <c r="O3" s="140" t="s">
+        <v>171</v>
+      </c>
+      <c r="P3" s="135" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1">
+      <c r="A4" s="187"/>
+      <c r="B4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="176"/>
-      <c r="F3" s="177" t="s">
+      <c r="C4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="173" t="s">
-        <v>192</v>
-      </c>
-      <c r="N3" s="52">
-        <v>0</v>
-      </c>
-      <c r="O3" s="113" t="s">
-        <v>181</v>
-      </c>
-      <c r="P3" s="113" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1">
-      <c r="A4" s="169"/>
-      <c r="B4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="178"/>
-      <c r="G4" s="174"/>
-      <c r="N4" s="52">
+      <c r="F4" s="196"/>
+      <c r="G4" s="192"/>
+      <c r="N4" s="139">
         <v>1</v>
       </c>
-      <c r="O4" s="113" t="s">
-        <v>182</v>
-      </c>
-      <c r="P4" s="113" t="s">
-        <v>170</v>
+      <c r="O4" s="140" t="s">
+        <v>172</v>
+      </c>
+      <c r="P4" s="135" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1">
       <c r="A5" s="20">
         <v>0</v>
       </c>
-      <c r="B5" s="170" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="128" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="129" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="52">
+      <c r="B5" s="188" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="190"/>
+      <c r="F5" s="126" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="127" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="139">
         <v>2</v>
       </c>
-      <c r="O5" s="113" t="s">
-        <v>183</v>
-      </c>
-      <c r="P5" s="113" t="s">
-        <v>172</v>
+      <c r="O5" s="140" t="s">
+        <v>200</v>
+      </c>
+      <c r="P5" s="135" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="30" customHeight="1">
       <c r="A6" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="170" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="123" t="s">
-        <v>193</v>
-      </c>
-      <c r="G6" s="116" t="s">
-        <v>194</v>
-      </c>
-      <c r="N6" s="52">
+      <c r="B6" s="188" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="190"/>
+      <c r="F6" s="121" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="114" t="s">
+        <v>180</v>
+      </c>
+      <c r="N6" s="139">
         <v>3</v>
       </c>
-      <c r="O6" s="113" t="s">
-        <v>184</v>
-      </c>
-      <c r="P6" s="113" t="s">
+      <c r="O6" s="140" t="s">
         <v>173</v>
+      </c>
+      <c r="P6" s="135" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1">
       <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="170" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="123" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="129" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="52"/>
-      <c r="O7" s="113" t="s">
-        <v>185</v>
-      </c>
-      <c r="P7" s="113" t="s">
+      <c r="B7" s="188" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="189"/>
+      <c r="D7" s="189"/>
+      <c r="E7" s="190"/>
+      <c r="F7" s="121" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="127" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="139"/>
+      <c r="O7" s="140" t="s">
         <v>174</v>
+      </c>
+      <c r="P7" s="135" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="26" customFormat="1" ht="84.75" customHeight="1">
@@ -4001,315 +4513,433 @@
         <v>3</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="170" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="172"/>
+        <v>38</v>
+      </c>
+      <c r="C8" s="188" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="190"/>
       <c r="E8" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="121" t="s">
-        <v>191</v>
-      </c>
-      <c r="G8" s="131" t="s">
-        <v>195</v>
-      </c>
-      <c r="N8" s="52">
+        <v>73</v>
+      </c>
+      <c r="F8" s="119" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" s="129" t="s">
+        <v>181</v>
+      </c>
+      <c r="N8" s="139">
         <v>5</v>
       </c>
-      <c r="O8" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="P8" s="113" t="s">
+      <c r="O8" s="140" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="45" customHeight="1">
+      <c r="P8" s="135" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="45" customHeight="1" thickBot="1">
       <c r="A9" s="20">
         <v>4</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="161" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="162"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="123" t="s">
-        <v>196</v>
-      </c>
-      <c r="G9" s="130" t="s">
-        <v>197</v>
-      </c>
-      <c r="N9" s="52">
+        <v>39</v>
+      </c>
+      <c r="C9" s="179" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="180"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="121" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" s="128" t="s">
+        <v>183</v>
+      </c>
+      <c r="N9" s="141">
         <v>6</v>
       </c>
-      <c r="O9" s="113" t="s">
-        <v>188</v>
-      </c>
-      <c r="P9" s="113" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="30" customHeight="1">
+      <c r="O9" s="142" t="s">
+        <v>176</v>
+      </c>
+      <c r="P9" s="135" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="30" customHeight="1" thickBot="1">
       <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="161" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="162"/>
-      <c r="D10" s="162"/>
-      <c r="E10" s="163"/>
-      <c r="F10" s="121" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="130" t="s">
-        <v>198</v>
-      </c>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="113" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="30" customHeight="1">
+      <c r="B10" s="179" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="180"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="119" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="128" t="s">
+        <v>184</v>
+      </c>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
+      <c r="P10" s="136" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="20">
         <v>6</v>
       </c>
-      <c r="B11" s="161" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="163"/>
-      <c r="D11" s="175" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="163"/>
-      <c r="F11" s="121" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="130" t="s">
-        <v>199</v>
-      </c>
+      <c r="B11" s="179" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="181"/>
+      <c r="D11" s="193" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="181"/>
+      <c r="F11" s="119" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="128" t="s">
+        <v>185</v>
+      </c>
+      <c r="N11" s="177" t="s">
+        <v>198</v>
+      </c>
+      <c r="O11" s="178"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1">
       <c r="A12" s="20">
         <v>7</v>
       </c>
-      <c r="B12" s="161" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="162"/>
-      <c r="D12" s="162"/>
-      <c r="E12" s="163"/>
-      <c r="F12" s="121" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="130" t="s">
-        <v>200</v>
+      <c r="B12" s="179" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="180"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="181"/>
+      <c r="F12" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="N12" s="137" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="138" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1" thickBot="1">
       <c r="A13" s="24">
         <v>8</v>
       </c>
-      <c r="B13" s="164" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
-      <c r="E13" s="166"/>
-      <c r="F13" s="125" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="130"/>
+      <c r="B13" s="182" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="183"/>
+      <c r="D13" s="183"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="123" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="128"/>
+      <c r="N13" s="133">
+        <v>0</v>
+      </c>
+      <c r="O13" s="133" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1">
+      <c r="N14" s="133">
+        <v>1</v>
+      </c>
+      <c r="O14" s="133" t="s">
+        <v>199</v>
+      </c>
       <c r="T14" s="42" t="s">
-        <v>176</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15" customHeight="1">
+      <c r="N15" s="133">
+        <v>2</v>
+      </c>
+      <c r="O15" s="143" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="26"/>
-      <c r="B16" s="167" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="167"/>
-      <c r="D16" s="167"/>
-      <c r="E16" s="167"/>
-      <c r="F16" s="114"/>
+      <c r="B16" s="185" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="185"/>
+      <c r="D16" s="185"/>
+      <c r="E16" s="185"/>
+      <c r="F16" s="112"/>
       <c r="G16" s="26"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1">
-      <c r="A17" s="168" t="s">
+      <c r="N16" s="133">
+        <v>3</v>
+      </c>
+      <c r="O16" s="133" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1">
+      <c r="A17" s="186" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="194" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="194"/>
+      <c r="D17" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="176" t="s">
+      <c r="E17" s="194"/>
+      <c r="F17" s="118"/>
+      <c r="G17" s="198" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="176"/>
-      <c r="D17" s="176" t="s">
+      <c r="N17" s="133"/>
+      <c r="O17" s="133" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1">
+      <c r="A18" s="197"/>
+      <c r="B18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="176"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="179" t="s">
+      <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1">
-      <c r="A18" s="169"/>
-      <c r="B18" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="127"/>
-      <c r="G18" s="180"/>
-    </row>
-    <row r="19" spans="1:14" s="19" customFormat="1" ht="30" customHeight="1">
+      <c r="F18" s="125"/>
+      <c r="G18" s="199"/>
+      <c r="N18" s="133">
+        <v>5</v>
+      </c>
+      <c r="O18" s="133" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="20">
         <v>0</v>
       </c>
-      <c r="B19" s="170" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
-      <c r="F19" s="124"/>
+      <c r="B19" s="188" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="189"/>
+      <c r="D19" s="189"/>
+      <c r="E19" s="190"/>
+      <c r="F19" s="122"/>
       <c r="G19" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1">
+        <v>47</v>
+      </c>
+      <c r="N19" s="133">
+        <v>6</v>
+      </c>
+      <c r="O19" s="133" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="19" customFormat="1" ht="15" customHeight="1">
       <c r="A20" s="20">
         <v>1</v>
       </c>
-      <c r="B20" s="170" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="171"/>
-      <c r="D20" s="171"/>
-      <c r="E20" s="172"/>
-      <c r="F20" s="124"/>
+      <c r="B20" s="188" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="189"/>
+      <c r="D20" s="189"/>
+      <c r="E20" s="190"/>
+      <c r="F20" s="122"/>
       <c r="G20" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1">
+        <v>46</v>
+      </c>
+      <c r="N20" s="130">
+        <v>7</v>
+      </c>
+      <c r="O20" s="144" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1">
       <c r="A21" s="20">
         <v>2</v>
       </c>
-      <c r="B21" s="170" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="171"/>
-      <c r="D21" s="171"/>
-      <c r="E21" s="172"/>
-      <c r="F21" s="124"/>
+      <c r="B21" s="188" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="189"/>
+      <c r="D21" s="189"/>
+      <c r="E21" s="190"/>
+      <c r="F21" s="122"/>
       <c r="G21" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="45" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="45" customHeight="1" thickBot="1">
       <c r="A22" s="20">
         <v>3</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="170" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="172"/>
+        <v>38</v>
+      </c>
+      <c r="C22" s="188" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="190"/>
       <c r="E22" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="123"/>
+        <v>73</v>
+      </c>
+      <c r="F22" s="121"/>
       <c r="G22" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="30" customHeight="1">
+        <v>74</v>
+      </c>
+      <c r="N22" s="177" t="s">
+        <v>206</v>
+      </c>
+      <c r="O22" s="178"/>
+    </row>
+    <row r="23" spans="1:15" ht="30" customHeight="1">
       <c r="A23" s="20">
         <v>4</v>
       </c>
       <c r="B23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="179" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="180"/>
+      <c r="E23" s="181"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="161" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="162"/>
-      <c r="E23" s="163"/>
-      <c r="F23" s="122"/>
-      <c r="G23" s="41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="30" customHeight="1">
+      <c r="N23" s="145" t="s">
+        <v>27</v>
+      </c>
+      <c r="O23" s="138" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="30" customHeight="1">
       <c r="A24" s="20">
         <v>5</v>
       </c>
-      <c r="B24" s="161" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="162"/>
-      <c r="D24" s="162"/>
-      <c r="E24" s="163"/>
-      <c r="F24" s="122"/>
+      <c r="B24" s="179" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="180"/>
+      <c r="D24" s="180"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="120"/>
       <c r="G24" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="N24" s="42"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1">
+        <v>71</v>
+      </c>
+      <c r="N24" s="133">
+        <v>0</v>
+      </c>
+      <c r="O24" s="133" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="20">
         <v>6</v>
       </c>
-      <c r="B25" s="161" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="162"/>
-      <c r="D25" s="162"/>
-      <c r="E25" s="163"/>
-      <c r="F25" s="122"/>
+      <c r="B25" s="179" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="180"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="120"/>
       <c r="G25" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+        <v>48</v>
+      </c>
+      <c r="N25" s="133">
+        <v>1</v>
+      </c>
+      <c r="O25" s="133" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
       <c r="A26" s="24">
         <v>7</v>
       </c>
-      <c r="B26" s="164" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="165"/>
-      <c r="D26" s="165"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="126"/>
+      <c r="B26" s="182" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="183"/>
+      <c r="D26" s="183"/>
+      <c r="E26" s="184"/>
+      <c r="F26" s="124"/>
       <c r="G26" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1"/>
+        <v>49</v>
+      </c>
+      <c r="N26" s="133">
+        <v>2</v>
+      </c>
+      <c r="O26" s="143" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1">
+      <c r="N27" s="133">
+        <v>3</v>
+      </c>
+      <c r="O27" s="133" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1">
+      <c r="N28" s="133"/>
+      <c r="O28" s="133" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1">
+      <c r="N29" s="133">
+        <v>5</v>
+      </c>
+      <c r="O29" s="133" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1">
+      <c r="N30" s="133">
+        <v>6</v>
+      </c>
+      <c r="O30" s="133" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1">
+      <c r="N31" s="130">
+        <v>7</v>
+      </c>
+      <c r="O31" s="144" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1"/>
     <row r="33" ht="30" customHeight="1"/>
     <row r="34" ht="30" customHeight="1"/>
     <row r="35" ht="47.25" customHeight="1"/>
@@ -5278,7 +5908,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="32">
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
@@ -5291,23 +5921,26 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="B24:E24"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:E9"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -5331,15 +5964,15 @@
     <row r="2" spans="2:3" ht="14.7" thickBot="1"/>
     <row r="3" spans="2:3">
       <c r="B3" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="29.1" thickBot="1">
       <c r="B4" s="38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="39">
         <v>43579</v>
@@ -5347,58 +5980,58 @@
     </row>
     <row r="5" spans="2:3" ht="14.7" thickBot="1">
       <c r="B5" s="36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:3">
@@ -5495,8 +6128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5510,35 +6143,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1">
-      <c r="B2" s="147" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="G2" s="181" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
+      <c r="B2" s="162" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="G2" s="200" t="s">
+        <v>192</v>
+      </c>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" s="49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H3" s="50" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:9">
@@ -5546,10 +6179,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E4" s="40"/>
       <c r="F4" s="40"/>
@@ -5560,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="56" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -5568,10 +6201,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E5" s="40"/>
       <c r="F5" s="40"/>
@@ -5582,7 +6215,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="28.8">
@@ -5590,10 +6223,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E6" s="40"/>
       <c r="F6" s="40"/>
@@ -5601,10 +6234,10 @@
         <v>2</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -5612,10 +6245,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="44" t="s">
         <v>87</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>90</v>
       </c>
       <c r="E7" s="40"/>
       <c r="F7" s="40"/>
@@ -5624,7 +6257,7 @@
       </c>
       <c r="H7" s="45"/>
       <c r="I7" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -5632,10 +6265,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E8" s="40"/>
       <c r="F8" s="40"/>
@@ -5644,7 +6277,7 @@
       </c>
       <c r="H8" s="45"/>
       <c r="I8" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -5655,7 +6288,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E9" s="40"/>
       <c r="F9" s="40"/>
@@ -5666,7 +6299,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="46" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -5674,10 +6307,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
@@ -5685,10 +6318,10 @@
         <v>6</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I10" s="46" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -5696,10 +6329,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
@@ -5707,10 +6340,10 @@
         <v>7</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I11" s="46" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -5718,10 +6351,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
@@ -5729,10 +6362,10 @@
         <v>8</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I12" s="46" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="2:9">
@@ -5740,10 +6373,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="40"/>
@@ -5752,7 +6385,7 @@
       </c>
       <c r="H13" s="45"/>
       <c r="I13" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -5760,10 +6393,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E14" s="40"/>
       <c r="F14" s="40"/>
@@ -5772,7 +6405,7 @@
       </c>
       <c r="H14" s="45"/>
       <c r="I14" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -5780,10 +6413,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
@@ -5792,7 +6425,7 @@
       </c>
       <c r="H15" s="45"/>
       <c r="I15" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -5800,10 +6433,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
@@ -5811,10 +6444,10 @@
         <v>12</v>
       </c>
       <c r="H16" s="43" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I16" s="44" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="28.8">
@@ -5822,10 +6455,10 @@
         <v>13</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
@@ -5834,7 +6467,7 @@
       </c>
       <c r="H17" s="45"/>
       <c r="I17" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="28.8">
@@ -5842,10 +6475,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
@@ -5854,18 +6487,18 @@
       </c>
       <c r="H18" s="45"/>
       <c r="I18" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="20">
         <v>15</v>
       </c>
-      <c r="C19" s="119" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="118" t="s">
-        <v>189</v>
+      <c r="C19" s="117" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="116" t="s">
+        <v>209</v>
       </c>
       <c r="E19" s="40"/>
       <c r="F19" s="40"/>
@@ -5874,18 +6507,18 @@
       </c>
       <c r="H19" s="45"/>
       <c r="I19" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="20">
         <v>16</v>
       </c>
-      <c r="C20" s="117" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="118" t="s">
-        <v>190</v>
+      <c r="C20" s="115" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="116" t="s">
+        <v>208</v>
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
@@ -5894,7 +6527,7 @@
       </c>
       <c r="H20" s="45"/>
       <c r="I20" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -5903,7 +6536,7 @@
       </c>
       <c r="C21" s="43"/>
       <c r="D21" s="44" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
@@ -5912,7 +6545,7 @@
       </c>
       <c r="H21" s="45"/>
       <c r="I21" s="46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -5920,10 +6553,10 @@
         <v>18</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
@@ -5931,10 +6564,10 @@
         <v>18</v>
       </c>
       <c r="H22" s="45" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I22" s="46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -5942,10 +6575,10 @@
         <v>19</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E23" s="40"/>
       <c r="F23" s="40"/>
@@ -5953,10 +6586,10 @@
         <v>19</v>
       </c>
       <c r="H23" s="45" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I23" s="46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -5964,10 +6597,10 @@
         <v>20</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E24" s="40"/>
       <c r="F24" s="40"/>
@@ -5975,10 +6608,10 @@
         <v>20</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I24" s="44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="14.7" thickBot="1">
@@ -5989,7 +6622,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E25" s="40"/>
       <c r="F25" s="40"/>
@@ -6000,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="48" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="2:9">

</xml_diff>